<commit_message>
show total admin earning
</commit_message>
<xml_diff>
--- a/assets/excel/animal_requirement.xlsx
+++ b/assets/excel/animal_requirement.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26306"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="70" documentId="11_B6C6E078602ADFEBC5B548282F9AA1C23F68F002" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD0A63D4-6D84-458C-8849-76B3F2EC9AB3}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fineoutput\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92164510-689F-42C3-8F97-C412627704DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" tabRatio="602" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="602" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NS Dary Cattle 1.0" sheetId="8" r:id="rId1"/>
@@ -687,7 +692,7 @@
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="38">
+  <fonts count="38" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3231,11 +3236,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB413"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="1"/>
@@ -3252,7 +3257,7 @@
     <col min="55" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="1" customFormat="1" ht="13.5" thickBot="1">
+    <row r="1" spans="1:54" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="87"/>
       <c r="B1" s="87"/>
       <c r="C1" s="87"/>
@@ -3308,7 +3313,7 @@
       <c r="BA1" s="87"/>
       <c r="BB1" s="87"/>
     </row>
-    <row r="2" spans="1:54">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A2" s="87"/>
       <c r="B2" s="87"/>
       <c r="C2" s="87"/>
@@ -3364,7 +3369,7 @@
       <c r="BA2" s="87"/>
       <c r="BB2" s="87"/>
     </row>
-    <row r="3" spans="1:54" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="3" spans="1:54" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -3420,7 +3425,7 @@
       <c r="BA3" s="4"/>
       <c r="BB3" s="4"/>
     </row>
-    <row r="4" spans="1:54" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="4" spans="1:54" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -3476,7 +3481,7 @@
       <c r="BA4" s="4"/>
       <c r="BB4" s="4"/>
     </row>
-    <row r="5" spans="1:54" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="5" spans="1:54" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -3532,7 +3537,7 @@
       <c r="BA5" s="4"/>
       <c r="BB5" s="4"/>
     </row>
-    <row r="6" spans="1:54" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="6" spans="1:54" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -3588,7 +3593,7 @@
       <c r="BA6" s="4"/>
       <c r="BB6" s="4"/>
     </row>
-    <row r="7" spans="1:54" s="6" customFormat="1" ht="24.75" customHeight="1">
+    <row r="7" spans="1:54" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -3646,7 +3651,7 @@
       <c r="BA7" s="4"/>
       <c r="BB7" s="4"/>
     </row>
-    <row r="8" spans="1:54" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="8" spans="1:54" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -3704,7 +3709,7 @@
       <c r="BA8" s="4"/>
       <c r="BB8" s="4"/>
     </row>
-    <row r="9" spans="1:54" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="9" spans="1:54" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -3762,7 +3767,7 @@
       <c r="BA9" s="4"/>
       <c r="BB9" s="4"/>
     </row>
-    <row r="10" spans="1:54" s="6" customFormat="1" ht="18" customHeight="1">
+    <row r="10" spans="1:54" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -3818,7 +3823,7 @@
       <c r="BA10" s="4"/>
       <c r="BB10" s="4"/>
     </row>
-    <row r="11" spans="1:54" ht="15.75" customHeight="1">
+    <row r="11" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="87"/>
       <c r="B11" s="87"/>
       <c r="C11" s="87"/>
@@ -3876,7 +3881,7 @@
       <c r="BA11" s="87"/>
       <c r="BB11" s="87"/>
     </row>
-    <row r="12" spans="1:54" ht="15.75" customHeight="1">
+    <row r="12" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="87"/>
       <c r="B12" s="87"/>
       <c r="C12" s="87"/>
@@ -3934,7 +3939,7 @@
       <c r="BA12" s="87"/>
       <c r="BB12" s="87"/>
     </row>
-    <row r="13" spans="1:54" ht="15.75" customHeight="1">
+    <row r="13" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="87"/>
       <c r="B13" s="87"/>
       <c r="C13" s="87"/>
@@ -3992,7 +3997,7 @@
       <c r="BA13" s="87"/>
       <c r="BB13" s="87"/>
     </row>
-    <row r="14" spans="1:54" ht="15">
+    <row r="14" spans="1:54" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" s="87"/>
       <c r="B14" s="87"/>
       <c r="C14" s="87"/>
@@ -4050,7 +4055,7 @@
       <c r="BA14" s="87"/>
       <c r="BB14" s="87"/>
     </row>
-    <row r="15" spans="1:54" ht="13.5">
+    <row r="15" spans="1:54" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A15" s="87"/>
       <c r="B15" s="87"/>
       <c r="C15" s="87"/>
@@ -4108,7 +4113,7 @@
       <c r="BA15" s="87"/>
       <c r="BB15" s="87"/>
     </row>
-    <row r="16" spans="1:54" ht="13.5">
+    <row r="16" spans="1:54" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A16" s="87"/>
       <c r="B16" s="87"/>
       <c r="C16" s="87"/>
@@ -4164,7 +4169,7 @@
       <c r="BA16" s="87"/>
       <c r="BB16" s="87"/>
     </row>
-    <row r="17" spans="1:54" ht="23.25">
+    <row r="17" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A17" s="87"/>
       <c r="B17" s="87"/>
       <c r="C17" s="87"/>
@@ -4222,7 +4227,7 @@
       <c r="BA17" s="87"/>
       <c r="BB17" s="87"/>
     </row>
-    <row r="18" spans="1:54">
+    <row r="18" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A18" s="87"/>
       <c r="B18" s="87"/>
       <c r="C18" s="87"/>
@@ -4278,7 +4283,7 @@
       <c r="BA18" s="87"/>
       <c r="BB18" s="87"/>
     </row>
-    <row r="19" spans="1:54" ht="15" customHeight="1">
+    <row r="19" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="87"/>
       <c r="B19" s="87"/>
       <c r="C19" s="87"/>
@@ -4336,7 +4341,7 @@
       <c r="BA19" s="87"/>
       <c r="BB19" s="87"/>
     </row>
-    <row r="20" spans="1:54" ht="15" customHeight="1">
+    <row r="20" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="87"/>
       <c r="B20" s="87"/>
       <c r="C20" s="87"/>
@@ -4392,7 +4397,7 @@
       <c r="BA20" s="87"/>
       <c r="BB20" s="87"/>
     </row>
-    <row r="21" spans="1:54" ht="15" customHeight="1">
+    <row r="21" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="87"/>
       <c r="B21" s="87"/>
       <c r="C21" s="87"/>
@@ -4458,7 +4463,7 @@
       <c r="BA21" s="87"/>
       <c r="BB21" s="87"/>
     </row>
-    <row r="22" spans="1:54" ht="15" customHeight="1">
+    <row r="22" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="87"/>
       <c r="B22" s="87"/>
       <c r="C22" s="87"/>
@@ -4524,7 +4529,7 @@
       <c r="BA22" s="87"/>
       <c r="BB22" s="87"/>
     </row>
-    <row r="23" spans="1:54" ht="15" customHeight="1">
+    <row r="23" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="87"/>
       <c r="B23" s="87"/>
       <c r="C23" s="87"/>
@@ -4592,7 +4597,7 @@
       <c r="BA23" s="87"/>
       <c r="BB23" s="87"/>
     </row>
-    <row r="24" spans="1:54" ht="15" customHeight="1">
+    <row r="24" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="87"/>
       <c r="B24" s="87"/>
       <c r="C24" s="87"/>
@@ -4660,7 +4665,7 @@
       <c r="BA24" s="87"/>
       <c r="BB24" s="87"/>
     </row>
-    <row r="25" spans="1:54" ht="15" customHeight="1">
+    <row r="25" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="87"/>
       <c r="B25" s="87"/>
       <c r="C25" s="87"/>
@@ -4728,7 +4733,7 @@
       <c r="BA25" s="87"/>
       <c r="BB25" s="87"/>
     </row>
-    <row r="26" spans="1:54" ht="15" customHeight="1">
+    <row r="26" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="87"/>
       <c r="B26" s="87"/>
       <c r="C26" s="87"/>
@@ -4795,7 +4800,7 @@
       <c r="BA26" s="87"/>
       <c r="BB26" s="87"/>
     </row>
-    <row r="27" spans="1:54" ht="18" customHeight="1">
+    <row r="27" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="87"/>
       <c r="B27" s="87"/>
       <c r="C27" s="87"/>
@@ -4864,7 +4869,7 @@
       <c r="BA27" s="87"/>
       <c r="BB27" s="87"/>
     </row>
-    <row r="28" spans="1:54" ht="15" customHeight="1">
+    <row r="28" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="87"/>
       <c r="B28" s="87"/>
       <c r="C28" s="87"/>
@@ -4926,7 +4931,7 @@
       <c r="BA28" s="87"/>
       <c r="BB28" s="87"/>
     </row>
-    <row r="29" spans="1:54" ht="15" customHeight="1">
+    <row r="29" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="87"/>
       <c r="B29" s="87"/>
       <c r="C29" s="87"/>
@@ -4982,7 +4987,7 @@
       <c r="BA29" s="87"/>
       <c r="BB29" s="87"/>
     </row>
-    <row r="30" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="30" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="87"/>
       <c r="B30" s="87"/>
       <c r="C30" s="87"/>
@@ -5040,7 +5045,7 @@
       <c r="BA30" s="87"/>
       <c r="BB30" s="87"/>
     </row>
-    <row r="31" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="31" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="87"/>
       <c r="B31" s="87"/>
       <c r="C31" s="87"/>
@@ -5096,7 +5101,7 @@
       <c r="BA31" s="87"/>
       <c r="BB31" s="87"/>
     </row>
-    <row r="32" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="32" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="87"/>
       <c r="B32" s="87"/>
       <c r="C32" s="87"/>
@@ -5166,7 +5171,7 @@
       <c r="BA32" s="87"/>
       <c r="BB32" s="87"/>
     </row>
-    <row r="33" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="33" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="87"/>
       <c r="B33" s="87"/>
       <c r="C33" s="87"/>
@@ -5232,7 +5237,7 @@
       <c r="BA33" s="87"/>
       <c r="BB33" s="87"/>
     </row>
-    <row r="34" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="34" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="87"/>
       <c r="B34" s="87"/>
       <c r="C34" s="87"/>
@@ -5288,7 +5293,7 @@
       <c r="BA34" s="87"/>
       <c r="BB34" s="87"/>
     </row>
-    <row r="35" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="35" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="87"/>
       <c r="B35" s="87"/>
       <c r="C35" s="87"/>
@@ -5346,7 +5351,7 @@
       <c r="BA35" s="87"/>
       <c r="BB35" s="87"/>
     </row>
-    <row r="36" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="36" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="87"/>
       <c r="B36" s="87"/>
       <c r="C36" s="87"/>
@@ -5402,7 +5407,7 @@
       <c r="BA36" s="87"/>
       <c r="BB36" s="87"/>
     </row>
-    <row r="37" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="37" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="87"/>
       <c r="B37" s="87"/>
       <c r="C37" s="87"/>
@@ -5462,7 +5467,7 @@
       <c r="BA37" s="87"/>
       <c r="BB37" s="87"/>
     </row>
-    <row r="38" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="38" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="87"/>
       <c r="B38" s="87"/>
       <c r="C38" s="87"/>
@@ -5532,7 +5537,7 @@
       <c r="BA38" s="87"/>
       <c r="BB38" s="87"/>
     </row>
-    <row r="39" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="39" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="87"/>
       <c r="B39" s="87"/>
       <c r="C39" s="87"/>
@@ -5602,7 +5607,7 @@
       <c r="BA39" s="87"/>
       <c r="BB39" s="87"/>
     </row>
-    <row r="40" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="40" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="87"/>
       <c r="B40" s="87"/>
       <c r="C40" s="87"/>
@@ -5672,7 +5677,7 @@
       <c r="BA40" s="87"/>
       <c r="BB40" s="87"/>
     </row>
-    <row r="41" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="41" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="87"/>
       <c r="B41" s="87"/>
       <c r="C41" s="87"/>
@@ -5742,7 +5747,7 @@
       <c r="BA41" s="87"/>
       <c r="BB41" s="87"/>
     </row>
-    <row r="42" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="42" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="87"/>
       <c r="B42" s="87"/>
       <c r="C42" s="87"/>
@@ -5812,7 +5817,7 @@
       <c r="BA42" s="87"/>
       <c r="BB42" s="87"/>
     </row>
-    <row r="43" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="43" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="87"/>
       <c r="B43" s="87"/>
       <c r="C43" s="87"/>
@@ -5882,7 +5887,7 @@
       <c r="BA43" s="87"/>
       <c r="BB43" s="87"/>
     </row>
-    <row r="44" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="44" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="87"/>
       <c r="B44" s="87"/>
       <c r="C44" s="87"/>
@@ -5952,7 +5957,7 @@
       <c r="BA44" s="87"/>
       <c r="BB44" s="87"/>
     </row>
-    <row r="45" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="45" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="87"/>
       <c r="B45" s="87"/>
       <c r="C45" s="87"/>
@@ -6022,7 +6027,7 @@
       <c r="BA45" s="87"/>
       <c r="BB45" s="87"/>
     </row>
-    <row r="46" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="46" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="87"/>
       <c r="B46" s="87"/>
       <c r="C46" s="87"/>
@@ -6085,7 +6090,7 @@
       <c r="BA46" s="87"/>
       <c r="BB46" s="87"/>
     </row>
-    <row r="47" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="47" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="87"/>
       <c r="B47" s="87"/>
       <c r="C47" s="87"/>
@@ -6147,7 +6152,7 @@
       <c r="BA47" s="87"/>
       <c r="BB47" s="87"/>
     </row>
-    <row r="48" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="48" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="87"/>
       <c r="B48" s="87"/>
       <c r="C48" s="87"/>
@@ -6210,7 +6215,7 @@
       <c r="BA48" s="87"/>
       <c r="BB48" s="87"/>
     </row>
-    <row r="49" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="49" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="87"/>
       <c r="B49" s="87"/>
       <c r="C49" s="87"/>
@@ -6266,7 +6271,7 @@
       <c r="BA49" s="87"/>
       <c r="BB49" s="87"/>
     </row>
-    <row r="50" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="50" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="87"/>
       <c r="B50" s="87"/>
       <c r="C50" s="87"/>
@@ -6326,7 +6331,7 @@
       <c r="BA50" s="87"/>
       <c r="BB50" s="87"/>
     </row>
-    <row r="51" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="51" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="87"/>
       <c r="B51" s="87"/>
       <c r="C51" s="87"/>
@@ -6396,7 +6401,7 @@
       <c r="BA51" s="87"/>
       <c r="BB51" s="87"/>
     </row>
-    <row r="52" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="52" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="87"/>
       <c r="B52" s="87"/>
       <c r="C52" s="87"/>
@@ -6466,7 +6471,7 @@
       <c r="BA52" s="87"/>
       <c r="BB52" s="87"/>
     </row>
-    <row r="53" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="53" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="87"/>
       <c r="B53" s="87"/>
       <c r="C53" s="87"/>
@@ -6536,7 +6541,7 @@
       <c r="BA53" s="87"/>
       <c r="BB53" s="87"/>
     </row>
-    <row r="54" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="54" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="87"/>
       <c r="B54" s="87"/>
       <c r="C54" s="87"/>
@@ -6606,7 +6611,7 @@
       <c r="BA54" s="87"/>
       <c r="BB54" s="87"/>
     </row>
-    <row r="55" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="55" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="87"/>
       <c r="B55" s="87"/>
       <c r="C55" s="87"/>
@@ -6676,7 +6681,7 @@
       <c r="BA55" s="87"/>
       <c r="BB55" s="87"/>
     </row>
-    <row r="56" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="56" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="87"/>
       <c r="B56" s="87"/>
       <c r="C56" s="87"/>
@@ -6745,7 +6750,7 @@
       <c r="BA56" s="87"/>
       <c r="BB56" s="87"/>
     </row>
-    <row r="57" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="57" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="87"/>
       <c r="B57" s="87"/>
       <c r="C57" s="87"/>
@@ -6815,7 +6820,7 @@
       <c r="BA57" s="87"/>
       <c r="BB57" s="87"/>
     </row>
-    <row r="58" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="58" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="87"/>
       <c r="B58" s="87"/>
       <c r="C58" s="87"/>
@@ -6884,7 +6889,7 @@
       <c r="BA58" s="87"/>
       <c r="BB58" s="87"/>
     </row>
-    <row r="59" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="59" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="87"/>
       <c r="B59" s="87"/>
       <c r="C59" s="87"/>
@@ -6954,7 +6959,7 @@
       <c r="BA59" s="87"/>
       <c r="BB59" s="87"/>
     </row>
-    <row r="60" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="60" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="87"/>
       <c r="B60" s="87"/>
       <c r="C60" s="87"/>
@@ -7023,7 +7028,7 @@
       <c r="BA60" s="87"/>
       <c r="BB60" s="87"/>
     </row>
-    <row r="61" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="61" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="87"/>
       <c r="B61" s="87"/>
       <c r="C61" s="87"/>
@@ -7093,7 +7098,7 @@
       <c r="BA61" s="87"/>
       <c r="BB61" s="87"/>
     </row>
-    <row r="62" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="62" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="87"/>
       <c r="B62" s="87"/>
       <c r="C62" s="87"/>
@@ -7162,7 +7167,7 @@
       <c r="BA62" s="87"/>
       <c r="BB62" s="87"/>
     </row>
-    <row r="63" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="63" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="87"/>
       <c r="B63" s="87"/>
       <c r="C63" s="87"/>
@@ -7225,7 +7230,7 @@
       <c r="BA63" s="87"/>
       <c r="BB63" s="87"/>
     </row>
-    <row r="64" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="64" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="87"/>
       <c r="B64" s="87"/>
       <c r="C64" s="87"/>
@@ -7287,7 +7292,7 @@
       <c r="BA64" s="87"/>
       <c r="BB64" s="87"/>
     </row>
-    <row r="65" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="65" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="87"/>
       <c r="B65" s="87"/>
       <c r="C65" s="87"/>
@@ -7350,7 +7355,7 @@
       <c r="BA65" s="87"/>
       <c r="BB65" s="87"/>
     </row>
-    <row r="66" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="66" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="87"/>
       <c r="B66" s="87"/>
       <c r="C66" s="87"/>
@@ -7413,7 +7418,7 @@
       <c r="BA66" s="87"/>
       <c r="BB66" s="87"/>
     </row>
-    <row r="67" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="67" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="87"/>
       <c r="B67" s="87"/>
       <c r="C67" s="87"/>
@@ -7469,7 +7474,7 @@
       <c r="BA67" s="87"/>
       <c r="BB67" s="87"/>
     </row>
-    <row r="68" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="68" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="87"/>
       <c r="B68" s="87"/>
       <c r="C68" s="87"/>
@@ -7529,7 +7534,7 @@
       <c r="BA68" s="87"/>
       <c r="BB68" s="87"/>
     </row>
-    <row r="69" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="69" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="87"/>
       <c r="B69" s="87"/>
       <c r="C69" s="87"/>
@@ -7598,7 +7603,7 @@
       <c r="BA69" s="87"/>
       <c r="BB69" s="87"/>
     </row>
-    <row r="70" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="70" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="87"/>
       <c r="B70" s="87"/>
       <c r="C70" s="87"/>
@@ -7667,7 +7672,7 @@
       <c r="BA70" s="87"/>
       <c r="BB70" s="87"/>
     </row>
-    <row r="71" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="71" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="87"/>
       <c r="B71" s="87"/>
       <c r="C71" s="87"/>
@@ -7730,7 +7735,7 @@
       <c r="BA71" s="87"/>
       <c r="BB71" s="87"/>
     </row>
-    <row r="72" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="72" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="87"/>
       <c r="B72" s="87"/>
       <c r="C72" s="87"/>
@@ -7788,7 +7793,7 @@
       <c r="BA72" s="87"/>
       <c r="BB72" s="87"/>
     </row>
-    <row r="73" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="73" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="87"/>
       <c r="B73" s="87"/>
       <c r="C73" s="87"/>
@@ -7851,7 +7856,7 @@
       <c r="BA73" s="87"/>
       <c r="BB73" s="87"/>
     </row>
-    <row r="74" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="74" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="87"/>
       <c r="B74" s="87"/>
       <c r="C74" s="87"/>
@@ -7907,7 +7912,7 @@
       <c r="BA74" s="87"/>
       <c r="BB74" s="87"/>
     </row>
-    <row r="75" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="75" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="87"/>
       <c r="B75" s="87"/>
       <c r="C75" s="87"/>
@@ -7965,7 +7970,7 @@
       <c r="BA75" s="87"/>
       <c r="BB75" s="87"/>
     </row>
-    <row r="76" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="76" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="87"/>
       <c r="B76" s="87"/>
       <c r="C76" s="87"/>
@@ -8023,7 +8028,7 @@
       <c r="BA76" s="87"/>
       <c r="BB76" s="87"/>
     </row>
-    <row r="77" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="77" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="87"/>
       <c r="B77" s="87"/>
       <c r="C77" s="87"/>
@@ -8079,7 +8084,7 @@
       <c r="BA77" s="87"/>
       <c r="BB77" s="87"/>
     </row>
-    <row r="78" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="78" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="87"/>
       <c r="B78" s="87"/>
       <c r="C78" s="87"/>
@@ -8137,7 +8142,7 @@
       <c r="BA78" s="87"/>
       <c r="BB78" s="87"/>
     </row>
-    <row r="79" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="79" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="87"/>
       <c r="B79" s="87"/>
       <c r="C79" s="87"/>
@@ -8193,7 +8198,7 @@
       <c r="BA79" s="87"/>
       <c r="BB79" s="87"/>
     </row>
-    <row r="80" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="80" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="87"/>
       <c r="B80" s="87"/>
       <c r="C80" s="87"/>
@@ -8251,7 +8256,7 @@
       <c r="BA80" s="87"/>
       <c r="BB80" s="87"/>
     </row>
-    <row r="81" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="81" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="87"/>
       <c r="B81" s="87"/>
       <c r="C81" s="87"/>
@@ -8307,7 +8312,7 @@
       <c r="BA81" s="87"/>
       <c r="BB81" s="87"/>
     </row>
-    <row r="82" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="82" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="87"/>
       <c r="B82" s="87"/>
       <c r="C82" s="87"/>
@@ -8363,7 +8368,7 @@
       <c r="BA82" s="87"/>
       <c r="BB82" s="87"/>
     </row>
-    <row r="83" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" thickBot="1">
+    <row r="83" spans="1:54" s="19" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="87"/>
       <c r="B83" s="87"/>
       <c r="C83" s="87"/>
@@ -8419,7 +8424,7 @@
       <c r="BA83" s="87"/>
       <c r="BB83" s="87"/>
     </row>
-    <row r="84" spans="1:54" s="1" customFormat="1" ht="15" customHeight="1">
+    <row r="84" spans="1:54" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="87"/>
       <c r="B84" s="87"/>
       <c r="C84" s="87"/>
@@ -8475,7 +8480,7 @@
       <c r="BA84" s="87"/>
       <c r="BB84" s="87"/>
     </row>
-    <row r="85" spans="1:54" s="1" customFormat="1" ht="15" customHeight="1">
+    <row r="85" spans="1:54" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="87"/>
       <c r="B85" s="87"/>
       <c r="C85" s="87"/>
@@ -8531,7 +8536,7 @@
       <c r="BA85" s="87"/>
       <c r="BB85" s="87"/>
     </row>
-    <row r="86" spans="1:54" s="1" customFormat="1" ht="15" customHeight="1">
+    <row r="86" spans="1:54" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="87"/>
       <c r="B86" s="87"/>
       <c r="C86" s="87"/>
@@ -8587,7 +8592,7 @@
       <c r="BA86" s="87"/>
       <c r="BB86" s="87"/>
     </row>
-    <row r="87" spans="1:54" s="83" customFormat="1" ht="15" customHeight="1">
+    <row r="87" spans="1:54" s="83" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M87" s="84"/>
       <c r="N87" s="84"/>
       <c r="O87" s="84"/>
@@ -8614,7 +8619,7 @@
       <c r="AJ87" s="84"/>
       <c r="AK87" s="84"/>
     </row>
-    <row r="88" spans="1:54" s="83" customFormat="1" ht="15" customHeight="1">
+    <row r="88" spans="1:54" s="83" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K88" s="85"/>
       <c r="L88" s="85"/>
       <c r="M88" s="84"/>
@@ -8643,26 +8648,26 @@
       <c r="AJ88" s="84"/>
       <c r="AK88" s="84"/>
     </row>
-    <row r="89" spans="1:54" s="84" customFormat="1" ht="15" customHeight="1"/>
-    <row r="90" spans="1:54" s="51" customFormat="1" ht="15" customHeight="1"/>
-    <row r="91" spans="1:54" s="51" customFormat="1" ht="15" customHeight="1"/>
-    <row r="92" spans="1:54" s="51" customFormat="1" ht="15" customHeight="1"/>
-    <row r="93" spans="1:54" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="89" spans="1:54" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" spans="1:54" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" spans="1:54" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" spans="1:54" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" spans="1:54" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H93" s="53"/>
       <c r="I93" s="53"/>
     </row>
-    <row r="94" spans="1:54" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="94" spans="1:54" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H94" s="53"/>
       <c r="I94" s="53"/>
     </row>
-    <row r="95" spans="1:54" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="95" spans="1:54" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E95" s="53"/>
       <c r="F95" s="53"/>
       <c r="G95" s="53"/>
       <c r="H95" s="53"/>
       <c r="I95" s="53"/>
     </row>
-    <row r="96" spans="1:54" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="96" spans="1:54" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E96" s="52" t="s">
         <v>114</v>
       </c>
@@ -8671,14 +8676,14 @@
       <c r="H96" s="53"/>
       <c r="I96" s="53"/>
     </row>
-    <row r="97" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="97" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E97" s="52"/>
       <c r="F97" s="53"/>
       <c r="G97" s="53"/>
       <c r="H97" s="53"/>
       <c r="I97" s="53"/>
     </row>
-    <row r="98" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="98" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E98" s="53" t="s">
         <v>11</v>
       </c>
@@ -8689,7 +8694,7 @@
       <c r="H98" s="53"/>
       <c r="I98" s="53"/>
     </row>
-    <row r="99" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="99" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E99" s="53" t="s">
         <v>115</v>
       </c>
@@ -8700,14 +8705,14 @@
       <c r="H99" s="53"/>
       <c r="I99" s="53"/>
     </row>
-    <row r="100" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="100" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E100" s="53"/>
       <c r="F100" s="53"/>
       <c r="G100" s="53"/>
       <c r="H100" s="53"/>
       <c r="I100" s="53"/>
     </row>
-    <row r="101" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="101" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E101" s="54" t="s">
         <v>117</v>
       </c>
@@ -8716,7 +8721,7 @@
       <c r="H101" s="53"/>
       <c r="I101" s="53"/>
     </row>
-    <row r="102" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="102" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E102" s="55" t="s">
         <v>118</v>
       </c>
@@ -8730,7 +8735,7 @@
       </c>
       <c r="I102" s="53"/>
     </row>
-    <row r="103" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="103" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E103" s="55" t="s">
         <v>120</v>
       </c>
@@ -8742,7 +8747,7 @@
       <c r="H103" s="53"/>
       <c r="I103" s="53"/>
     </row>
-    <row r="104" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="104" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E104" s="55" t="s">
         <v>118</v>
       </c>
@@ -8754,7 +8759,7 @@
       <c r="H104" s="53"/>
       <c r="I104" s="53"/>
     </row>
-    <row r="105" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="105" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E105" s="55" t="s">
         <v>120</v>
       </c>
@@ -8766,35 +8771,35 @@
       <c r="H105" s="53"/>
       <c r="I105" s="53"/>
     </row>
-    <row r="106" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="106" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E106" s="53"/>
       <c r="F106" s="57"/>
       <c r="G106" s="53"/>
       <c r="H106" s="53"/>
       <c r="I106" s="53"/>
     </row>
-    <row r="107" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="107" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E107" s="53"/>
       <c r="F107" s="57"/>
       <c r="G107" s="53"/>
       <c r="H107" s="53"/>
       <c r="I107" s="53"/>
     </row>
-    <row r="108" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="108" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E108" s="53"/>
       <c r="F108" s="58"/>
       <c r="G108" s="53"/>
       <c r="H108" s="53"/>
       <c r="I108" s="53"/>
     </row>
-    <row r="109" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="109" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E109" s="53"/>
       <c r="F109" s="58"/>
       <c r="G109" s="53"/>
       <c r="H109" s="53"/>
       <c r="I109" s="53"/>
     </row>
-    <row r="110" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="110" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E110" s="54" t="s">
         <v>121</v>
       </c>
@@ -8803,7 +8808,7 @@
       <c r="H110" s="53"/>
       <c r="I110" s="53"/>
     </row>
-    <row r="111" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="111" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E111" s="53" t="s">
         <v>122</v>
       </c>
@@ -8816,7 +8821,7 @@
       </c>
       <c r="I111" s="53"/>
     </row>
-    <row r="112" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="112" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E112" s="53" t="s">
         <v>124</v>
       </c>
@@ -8829,7 +8834,7 @@
       </c>
       <c r="I112" s="53"/>
     </row>
-    <row r="113" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="113" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E113" s="53" t="s">
         <v>125</v>
       </c>
@@ -8842,7 +8847,7 @@
       </c>
       <c r="I113" s="53"/>
     </row>
-    <row r="114" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="114" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E114" s="53" t="s">
         <v>127</v>
       </c>
@@ -8855,7 +8860,7 @@
       </c>
       <c r="I114" s="53"/>
     </row>
-    <row r="115" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="115" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E115" s="53" t="s">
         <v>128</v>
       </c>
@@ -8869,7 +8874,7 @@
       <c r="I115" s="53"/>
       <c r="M115" s="59"/>
     </row>
-    <row r="116" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="116" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E116" s="53" t="s">
         <v>129</v>
       </c>
@@ -8882,7 +8887,7 @@
       </c>
       <c r="I116" s="53"/>
     </row>
-    <row r="117" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="117" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E117" s="53" t="s">
         <v>130</v>
       </c>
@@ -8895,7 +8900,7 @@
       </c>
       <c r="I117" s="53"/>
     </row>
-    <row r="118" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="118" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E118" s="60" t="s">
         <v>131</v>
       </c>
@@ -8908,13 +8913,13 @@
       </c>
       <c r="I118" s="53"/>
     </row>
-    <row r="119" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="119" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E119" s="60"/>
       <c r="F119" s="62"/>
       <c r="G119" s="57"/>
       <c r="I119" s="53"/>
     </row>
-    <row r="120" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="120" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E120" s="53" t="s">
         <v>133</v>
       </c>
@@ -8927,7 +8932,7 @@
       </c>
       <c r="I120" s="53"/>
     </row>
-    <row r="121" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="121" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E121" s="53" t="s">
         <v>134</v>
       </c>
@@ -8938,7 +8943,7 @@
       <c r="G121" s="53"/>
       <c r="I121" s="53"/>
     </row>
-    <row r="122" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="122" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E122" s="51" t="s">
         <v>135</v>
       </c>
@@ -8951,7 +8956,7 @@
       </c>
       <c r="I122" s="53"/>
     </row>
-    <row r="123" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="123" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E123" s="53" t="s">
         <v>136</v>
       </c>
@@ -8964,7 +8969,7 @@
       </c>
       <c r="I123" s="53"/>
     </row>
-    <row r="124" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="124" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E124" s="53" t="s">
         <v>137</v>
       </c>
@@ -8977,7 +8982,7 @@
       </c>
       <c r="I124" s="53"/>
     </row>
-    <row r="125" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="125" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E125" s="53" t="s">
         <v>138</v>
       </c>
@@ -8990,7 +8995,7 @@
       </c>
       <c r="I125" s="53"/>
     </row>
-    <row r="126" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="126" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E126" s="53" t="s">
         <v>139</v>
       </c>
@@ -9003,7 +9008,7 @@
       </c>
       <c r="I126" s="53"/>
     </row>
-    <row r="127" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="127" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E127" s="60" t="s">
         <v>140</v>
       </c>
@@ -9016,13 +9021,13 @@
       </c>
       <c r="I127" s="53"/>
     </row>
-    <row r="128" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="128" spans="5:13" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E128" s="60"/>
       <c r="F128" s="61"/>
       <c r="G128" s="60"/>
       <c r="I128" s="53"/>
     </row>
-    <row r="129" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="129" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E129" s="54" t="s">
         <v>141</v>
       </c>
@@ -9031,14 +9036,14 @@
       <c r="H129" s="64"/>
       <c r="I129" s="53"/>
     </row>
-    <row r="130" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="130" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E130" s="53"/>
       <c r="F130" s="53"/>
       <c r="G130" s="53"/>
       <c r="H130" s="53"/>
       <c r="I130" s="53"/>
     </row>
-    <row r="131" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="131" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E131" s="53" t="s">
         <v>142</v>
       </c>
@@ -9052,7 +9057,7 @@
       <c r="H131" s="53"/>
       <c r="I131" s="53"/>
     </row>
-    <row r="132" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="132" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E132" s="53" t="s">
         <v>144</v>
       </c>
@@ -9064,7 +9069,7 @@
       <c r="H132" s="57"/>
       <c r="I132" s="53"/>
     </row>
-    <row r="133" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="133" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E133" s="53" t="s">
         <v>145</v>
       </c>
@@ -9078,14 +9083,14 @@
       <c r="H133" s="65"/>
       <c r="I133" s="66"/>
     </row>
-    <row r="134" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="134" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E134" s="53"/>
       <c r="F134" s="56"/>
       <c r="G134" s="53"/>
       <c r="H134" s="65"/>
       <c r="I134" s="66"/>
     </row>
-    <row r="135" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="135" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E135" s="53" t="s">
         <v>146</v>
       </c>
@@ -9099,7 +9104,7 @@
       <c r="H135" s="65"/>
       <c r="I135" s="66"/>
     </row>
-    <row r="136" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="136" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E136" s="53" t="s">
         <v>147</v>
       </c>
@@ -9110,7 +9115,7 @@
       <c r="H136" s="68"/>
       <c r="I136" s="53"/>
     </row>
-    <row r="137" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="137" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E137" s="53" t="s">
         <v>148</v>
       </c>
@@ -9124,14 +9129,14 @@
       <c r="H137" s="68"/>
       <c r="I137" s="53"/>
     </row>
-    <row r="138" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="138" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E138" s="53"/>
       <c r="F138" s="56"/>
       <c r="G138" s="53"/>
       <c r="H138" s="68"/>
       <c r="I138" s="53"/>
     </row>
-    <row r="139" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="139" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E139" s="53" t="s">
         <v>149</v>
       </c>
@@ -9145,11 +9150,11 @@
       <c r="H139" s="68"/>
       <c r="I139" s="53"/>
     </row>
-    <row r="140" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="140" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H140" s="65"/>
       <c r="I140" s="53"/>
     </row>
-    <row r="141" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="141" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E141" s="60" t="s">
         <v>150</v>
       </c>
@@ -9163,16 +9168,16 @@
       <c r="H141" s="65"/>
       <c r="I141" s="53"/>
     </row>
-    <row r="142" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="142" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E142" s="53"/>
       <c r="F142" s="57"/>
       <c r="G142" s="71"/>
       <c r="H142" s="72"/>
       <c r="I142" s="53"/>
     </row>
-    <row r="143" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1"/>
-    <row r="144" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1"/>
-    <row r="145" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="143" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E145" s="51" t="s">
         <v>151</v>
       </c>
@@ -9184,7 +9189,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="146" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="146" spans="5:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E146" s="51" t="s">
         <v>152</v>
       </c>
@@ -9196,7 +9201,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="147" spans="5:9" s="51" customFormat="1">
+    <row r="147" spans="5:9" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E147" s="53" t="s">
         <v>153</v>
       </c>
@@ -9210,7 +9215,7 @@
       <c r="H147" s="74"/>
       <c r="I147" s="53"/>
     </row>
-    <row r="148" spans="5:9" s="51" customFormat="1">
+    <row r="148" spans="5:9" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E148" s="53" t="s">
         <v>154</v>
       </c>
@@ -9224,7 +9229,7 @@
       <c r="H148" s="72"/>
       <c r="I148" s="53"/>
     </row>
-    <row r="149" spans="5:9" s="51" customFormat="1">
+    <row r="149" spans="5:9" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E149" s="53" t="s">
         <v>155</v>
       </c>
@@ -9238,7 +9243,7 @@
       <c r="H149" s="72"/>
       <c r="I149" s="53"/>
     </row>
-    <row r="150" spans="5:9" s="51" customFormat="1">
+    <row r="150" spans="5:9" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E150" s="53" t="s">
         <v>157</v>
       </c>
@@ -9249,7 +9254,7 @@
       <c r="H150" s="72"/>
       <c r="I150" s="53"/>
     </row>
-    <row r="151" spans="5:9" s="51" customFormat="1">
+    <row r="151" spans="5:9" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E151" s="51" t="s">
         <v>158</v>
       </c>
@@ -9261,54 +9266,54 @@
         <v>159</v>
       </c>
     </row>
-    <row r="152" spans="5:9" s="51" customFormat="1">
+    <row r="152" spans="5:9" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F152" s="56"/>
     </row>
-    <row r="153" spans="5:9" s="84" customFormat="1">
+    <row r="153" spans="5:9" s="84" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F153" s="86"/>
     </row>
-    <row r="154" spans="5:9" s="84" customFormat="1"/>
-    <row r="155" spans="5:9" s="84" customFormat="1"/>
-    <row r="156" spans="5:9" s="84" customFormat="1"/>
-    <row r="157" spans="5:9" s="84" customFormat="1"/>
-    <row r="158" spans="5:9" s="84" customFormat="1"/>
-    <row r="159" spans="5:9" s="84" customFormat="1"/>
-    <row r="160" spans="5:9" s="84" customFormat="1"/>
-    <row r="161" s="84" customFormat="1"/>
-    <row r="162" s="84" customFormat="1"/>
-    <row r="163" s="84" customFormat="1"/>
-    <row r="164" s="84" customFormat="1"/>
-    <row r="165" s="84" customFormat="1"/>
-    <row r="166" s="84" customFormat="1"/>
-    <row r="167" s="84" customFormat="1"/>
-    <row r="168" s="84" customFormat="1"/>
-    <row r="169" s="84" customFormat="1"/>
-    <row r="170" s="84" customFormat="1"/>
-    <row r="171" s="84" customFormat="1"/>
-    <row r="172" s="84" customFormat="1"/>
-    <row r="173" s="84" customFormat="1"/>
-    <row r="174" s="84" customFormat="1"/>
-    <row r="175" s="84" customFormat="1"/>
-    <row r="176" s="84" customFormat="1"/>
-    <row r="177" s="84" customFormat="1"/>
-    <row r="178" s="84" customFormat="1"/>
-    <row r="179" s="84" customFormat="1"/>
-    <row r="180" s="84" customFormat="1"/>
-    <row r="181" s="84" customFormat="1"/>
-    <row r="182" s="84" customFormat="1"/>
-    <row r="183" s="84" customFormat="1"/>
-    <row r="184" s="84" customFormat="1"/>
-    <row r="185" s="84" customFormat="1"/>
-    <row r="186" s="84" customFormat="1"/>
-    <row r="187" s="84" customFormat="1"/>
-    <row r="188" s="84" customFormat="1"/>
-    <row r="189" s="84" customFormat="1"/>
-    <row r="190" s="84" customFormat="1"/>
-    <row r="191" s="84" customFormat="1"/>
-    <row r="192" s="84" customFormat="1"/>
-    <row r="193" spans="5:37" s="84" customFormat="1"/>
-    <row r="194" spans="5:37" s="84" customFormat="1"/>
-    <row r="195" spans="5:37" s="83" customFormat="1">
+    <row r="154" spans="5:9" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="155" spans="5:9" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="156" spans="5:9" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="157" spans="5:9" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="158" spans="5:9" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="159" spans="5:9" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="160" spans="5:9" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="161" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="162" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="163" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="164" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="165" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="166" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="167" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="168" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="169" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="170" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="171" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="172" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="173" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="174" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="175" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="176" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="177" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="178" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="179" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="180" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="181" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="182" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="183" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="184" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="185" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="186" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="187" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="188" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="189" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="190" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="191" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="192" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="193" spans="5:37" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="194" spans="5:37" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="195" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E195" s="84"/>
       <c r="F195" s="84"/>
       <c r="G195" s="84"/>
@@ -9343,7 +9348,7 @@
       <c r="AJ195" s="84"/>
       <c r="AK195" s="84"/>
     </row>
-    <row r="196" spans="5:37" s="83" customFormat="1">
+    <row r="196" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E196" s="84"/>
       <c r="F196" s="84"/>
       <c r="G196" s="84"/>
@@ -9378,7 +9383,7 @@
       <c r="AJ196" s="84"/>
       <c r="AK196" s="84"/>
     </row>
-    <row r="197" spans="5:37" s="83" customFormat="1">
+    <row r="197" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E197" s="84"/>
       <c r="F197" s="84"/>
       <c r="G197" s="84"/>
@@ -9413,7 +9418,7 @@
       <c r="AJ197" s="84"/>
       <c r="AK197" s="84"/>
     </row>
-    <row r="198" spans="5:37" s="83" customFormat="1">
+    <row r="198" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E198" s="84"/>
       <c r="F198" s="84"/>
       <c r="G198" s="84"/>
@@ -9448,7 +9453,7 @@
       <c r="AJ198" s="84"/>
       <c r="AK198" s="84"/>
     </row>
-    <row r="199" spans="5:37" s="83" customFormat="1">
+    <row r="199" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E199" s="84"/>
       <c r="F199" s="84"/>
       <c r="G199" s="84"/>
@@ -9483,7 +9488,7 @@
       <c r="AJ199" s="84"/>
       <c r="AK199" s="84"/>
     </row>
-    <row r="200" spans="5:37" s="83" customFormat="1">
+    <row r="200" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E200" s="84"/>
       <c r="F200" s="84"/>
       <c r="G200" s="84"/>
@@ -9518,7 +9523,7 @@
       <c r="AJ200" s="84"/>
       <c r="AK200" s="84"/>
     </row>
-    <row r="201" spans="5:37" s="83" customFormat="1">
+    <row r="201" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E201" s="84"/>
       <c r="F201" s="84"/>
       <c r="G201" s="84"/>
@@ -9553,7 +9558,7 @@
       <c r="AJ201" s="84"/>
       <c r="AK201" s="84"/>
     </row>
-    <row r="202" spans="5:37" s="83" customFormat="1">
+    <row r="202" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E202" s="84"/>
       <c r="F202" s="84"/>
       <c r="G202" s="84"/>
@@ -9588,7 +9593,7 @@
       <c r="AJ202" s="84"/>
       <c r="AK202" s="84"/>
     </row>
-    <row r="203" spans="5:37" s="83" customFormat="1">
+    <row r="203" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E203" s="84"/>
       <c r="F203" s="84"/>
       <c r="G203" s="84"/>
@@ -9623,7 +9628,7 @@
       <c r="AJ203" s="84"/>
       <c r="AK203" s="84"/>
     </row>
-    <row r="204" spans="5:37" s="83" customFormat="1">
+    <row r="204" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E204" s="84"/>
       <c r="F204" s="84"/>
       <c r="G204" s="84"/>
@@ -9658,7 +9663,7 @@
       <c r="AJ204" s="84"/>
       <c r="AK204" s="84"/>
     </row>
-    <row r="205" spans="5:37" s="83" customFormat="1">
+    <row r="205" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E205" s="84"/>
       <c r="F205" s="84"/>
       <c r="G205" s="84"/>
@@ -9693,7 +9698,7 @@
       <c r="AJ205" s="84"/>
       <c r="AK205" s="84"/>
     </row>
-    <row r="206" spans="5:37" s="83" customFormat="1">
+    <row r="206" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E206" s="84"/>
       <c r="F206" s="84"/>
       <c r="G206" s="84"/>
@@ -9728,7 +9733,7 @@
       <c r="AJ206" s="84"/>
       <c r="AK206" s="84"/>
     </row>
-    <row r="207" spans="5:37" s="83" customFormat="1">
+    <row r="207" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E207" s="84"/>
       <c r="F207" s="84"/>
       <c r="G207" s="84"/>
@@ -9763,7 +9768,7 @@
       <c r="AJ207" s="84"/>
       <c r="AK207" s="84"/>
     </row>
-    <row r="208" spans="5:37" s="83" customFormat="1">
+    <row r="208" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E208" s="84"/>
       <c r="F208" s="84"/>
       <c r="G208" s="84"/>
@@ -9798,7 +9803,7 @@
       <c r="AJ208" s="84"/>
       <c r="AK208" s="84"/>
     </row>
-    <row r="209" spans="5:37" s="83" customFormat="1">
+    <row r="209" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E209" s="84"/>
       <c r="F209" s="84"/>
       <c r="G209" s="84"/>
@@ -9833,7 +9838,7 @@
       <c r="AJ209" s="84"/>
       <c r="AK209" s="84"/>
     </row>
-    <row r="210" spans="5:37" s="83" customFormat="1">
+    <row r="210" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E210" s="84"/>
       <c r="F210" s="84"/>
       <c r="G210" s="84"/>
@@ -9868,7 +9873,7 @@
       <c r="AJ210" s="84"/>
       <c r="AK210" s="84"/>
     </row>
-    <row r="211" spans="5:37" s="83" customFormat="1">
+    <row r="211" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E211" s="84"/>
       <c r="F211" s="84"/>
       <c r="G211" s="84"/>
@@ -9903,7 +9908,7 @@
       <c r="AJ211" s="84"/>
       <c r="AK211" s="84"/>
     </row>
-    <row r="212" spans="5:37" s="83" customFormat="1">
+    <row r="212" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E212" s="84"/>
       <c r="F212" s="84"/>
       <c r="G212" s="84"/>
@@ -9938,7 +9943,7 @@
       <c r="AJ212" s="84"/>
       <c r="AK212" s="84"/>
     </row>
-    <row r="213" spans="5:37" s="83" customFormat="1">
+    <row r="213" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E213" s="84"/>
       <c r="F213" s="84"/>
       <c r="G213" s="84"/>
@@ -9973,7 +9978,7 @@
       <c r="AJ213" s="84"/>
       <c r="AK213" s="84"/>
     </row>
-    <row r="214" spans="5:37" s="83" customFormat="1">
+    <row r="214" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E214" s="84"/>
       <c r="F214" s="84"/>
       <c r="G214" s="84"/>
@@ -10008,7 +10013,7 @@
       <c r="AJ214" s="84"/>
       <c r="AK214" s="84"/>
     </row>
-    <row r="215" spans="5:37" s="83" customFormat="1">
+    <row r="215" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E215" s="84"/>
       <c r="F215" s="84"/>
       <c r="G215" s="84"/>
@@ -10043,7 +10048,7 @@
       <c r="AJ215" s="84"/>
       <c r="AK215" s="84"/>
     </row>
-    <row r="216" spans="5:37" s="83" customFormat="1">
+    <row r="216" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E216" s="84"/>
       <c r="F216" s="84"/>
       <c r="G216" s="84"/>
@@ -10078,7 +10083,7 @@
       <c r="AJ216" s="84"/>
       <c r="AK216" s="84"/>
     </row>
-    <row r="217" spans="5:37" s="83" customFormat="1">
+    <row r="217" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E217" s="84"/>
       <c r="F217" s="84"/>
       <c r="G217" s="84"/>
@@ -10113,7 +10118,7 @@
       <c r="AJ217" s="84"/>
       <c r="AK217" s="84"/>
     </row>
-    <row r="218" spans="5:37" s="83" customFormat="1">
+    <row r="218" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E218" s="84"/>
       <c r="F218" s="84"/>
       <c r="G218" s="84"/>
@@ -10148,7 +10153,7 @@
       <c r="AJ218" s="84"/>
       <c r="AK218" s="84"/>
     </row>
-    <row r="219" spans="5:37" s="83" customFormat="1">
+    <row r="219" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E219" s="84"/>
       <c r="F219" s="84"/>
       <c r="G219" s="84"/>
@@ -10183,7 +10188,7 @@
       <c r="AJ219" s="84"/>
       <c r="AK219" s="84"/>
     </row>
-    <row r="220" spans="5:37" s="83" customFormat="1">
+    <row r="220" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E220" s="84"/>
       <c r="F220" s="84"/>
       <c r="G220" s="84"/>
@@ -10218,7 +10223,7 @@
       <c r="AJ220" s="84"/>
       <c r="AK220" s="84"/>
     </row>
-    <row r="221" spans="5:37" s="83" customFormat="1">
+    <row r="221" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E221" s="84"/>
       <c r="F221" s="84"/>
       <c r="G221" s="84"/>
@@ -10253,7 +10258,7 @@
       <c r="AJ221" s="84"/>
       <c r="AK221" s="84"/>
     </row>
-    <row r="222" spans="5:37" s="83" customFormat="1">
+    <row r="222" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E222" s="84"/>
       <c r="F222" s="84"/>
       <c r="G222" s="84"/>
@@ -10288,7 +10293,7 @@
       <c r="AJ222" s="84"/>
       <c r="AK222" s="84"/>
     </row>
-    <row r="223" spans="5:37" s="83" customFormat="1">
+    <row r="223" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E223" s="84"/>
       <c r="F223" s="84"/>
       <c r="G223" s="84"/>
@@ -10323,7 +10328,7 @@
       <c r="AJ223" s="84"/>
       <c r="AK223" s="84"/>
     </row>
-    <row r="224" spans="5:37" s="83" customFormat="1">
+    <row r="224" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E224" s="84"/>
       <c r="F224" s="84"/>
       <c r="G224" s="84"/>
@@ -10358,7 +10363,7 @@
       <c r="AJ224" s="84"/>
       <c r="AK224" s="84"/>
     </row>
-    <row r="225" spans="5:37" s="83" customFormat="1">
+    <row r="225" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E225" s="84"/>
       <c r="F225" s="84"/>
       <c r="G225" s="84"/>
@@ -10393,7 +10398,7 @@
       <c r="AJ225" s="84"/>
       <c r="AK225" s="84"/>
     </row>
-    <row r="226" spans="5:37" s="83" customFormat="1">
+    <row r="226" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E226" s="84"/>
       <c r="F226" s="84"/>
       <c r="G226" s="84"/>
@@ -10428,7 +10433,7 @@
       <c r="AJ226" s="84"/>
       <c r="AK226" s="84"/>
     </row>
-    <row r="227" spans="5:37" s="83" customFormat="1">
+    <row r="227" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E227" s="84"/>
       <c r="F227" s="84"/>
       <c r="G227" s="84"/>
@@ -10463,7 +10468,7 @@
       <c r="AJ227" s="84"/>
       <c r="AK227" s="84"/>
     </row>
-    <row r="228" spans="5:37" s="83" customFormat="1">
+    <row r="228" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E228" s="84"/>
       <c r="F228" s="84"/>
       <c r="G228" s="84"/>
@@ -10498,7 +10503,7 @@
       <c r="AJ228" s="84"/>
       <c r="AK228" s="84"/>
     </row>
-    <row r="229" spans="5:37" s="83" customFormat="1">
+    <row r="229" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E229" s="84"/>
       <c r="F229" s="84"/>
       <c r="G229" s="84"/>
@@ -10533,7 +10538,7 @@
       <c r="AJ229" s="84"/>
       <c r="AK229" s="84"/>
     </row>
-    <row r="230" spans="5:37" s="83" customFormat="1">
+    <row r="230" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E230" s="84"/>
       <c r="F230" s="84"/>
       <c r="G230" s="84"/>
@@ -10568,7 +10573,7 @@
       <c r="AJ230" s="84"/>
       <c r="AK230" s="84"/>
     </row>
-    <row r="231" spans="5:37" s="83" customFormat="1">
+    <row r="231" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E231" s="84"/>
       <c r="F231" s="84"/>
       <c r="G231" s="84"/>
@@ -10603,7 +10608,7 @@
       <c r="AJ231" s="84"/>
       <c r="AK231" s="84"/>
     </row>
-    <row r="232" spans="5:37" s="83" customFormat="1">
+    <row r="232" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E232" s="84"/>
       <c r="F232" s="84"/>
       <c r="G232" s="84"/>
@@ -10638,7 +10643,7 @@
       <c r="AJ232" s="84"/>
       <c r="AK232" s="84"/>
     </row>
-    <row r="233" spans="5:37" s="83" customFormat="1">
+    <row r="233" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E233" s="84"/>
       <c r="F233" s="84"/>
       <c r="G233" s="84"/>
@@ -10673,7 +10678,7 @@
       <c r="AJ233" s="84"/>
       <c r="AK233" s="84"/>
     </row>
-    <row r="234" spans="5:37" s="83" customFormat="1">
+    <row r="234" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E234" s="84"/>
       <c r="F234" s="84"/>
       <c r="G234" s="84"/>
@@ -10708,7 +10713,7 @@
       <c r="AJ234" s="84"/>
       <c r="AK234" s="84"/>
     </row>
-    <row r="235" spans="5:37" s="83" customFormat="1">
+    <row r="235" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E235" s="84"/>
       <c r="F235" s="84"/>
       <c r="G235" s="84"/>
@@ -10743,7 +10748,7 @@
       <c r="AJ235" s="84"/>
       <c r="AK235" s="84"/>
     </row>
-    <row r="236" spans="5:37" s="83" customFormat="1">
+    <row r="236" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E236" s="84"/>
       <c r="F236" s="84"/>
       <c r="G236" s="84"/>
@@ -10778,7 +10783,7 @@
       <c r="AJ236" s="84"/>
       <c r="AK236" s="84"/>
     </row>
-    <row r="237" spans="5:37" s="83" customFormat="1">
+    <row r="237" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E237" s="84"/>
       <c r="F237" s="84"/>
       <c r="G237" s="84"/>
@@ -10813,7 +10818,7 @@
       <c r="AJ237" s="84"/>
       <c r="AK237" s="84"/>
     </row>
-    <row r="238" spans="5:37" s="83" customFormat="1">
+    <row r="238" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E238" s="84"/>
       <c r="F238" s="84"/>
       <c r="G238" s="84"/>
@@ -10848,7 +10853,7 @@
       <c r="AJ238" s="84"/>
       <c r="AK238" s="84"/>
     </row>
-    <row r="239" spans="5:37" s="83" customFormat="1">
+    <row r="239" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E239" s="84"/>
       <c r="F239" s="84"/>
       <c r="G239" s="84"/>
@@ -10883,7 +10888,7 @@
       <c r="AJ239" s="84"/>
       <c r="AK239" s="84"/>
     </row>
-    <row r="240" spans="5:37" s="83" customFormat="1">
+    <row r="240" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E240" s="84"/>
       <c r="F240" s="84"/>
       <c r="G240" s="84"/>
@@ -10918,7 +10923,7 @@
       <c r="AJ240" s="84"/>
       <c r="AK240" s="84"/>
     </row>
-    <row r="241" spans="5:37" s="83" customFormat="1">
+    <row r="241" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E241" s="84"/>
       <c r="F241" s="84"/>
       <c r="G241" s="84"/>
@@ -10953,7 +10958,7 @@
       <c r="AJ241" s="84"/>
       <c r="AK241" s="84"/>
     </row>
-    <row r="242" spans="5:37" s="83" customFormat="1">
+    <row r="242" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E242" s="84"/>
       <c r="F242" s="84"/>
       <c r="G242" s="84"/>
@@ -10988,7 +10993,7 @@
       <c r="AJ242" s="84"/>
       <c r="AK242" s="84"/>
     </row>
-    <row r="243" spans="5:37" s="83" customFormat="1">
+    <row r="243" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E243" s="84"/>
       <c r="F243" s="84"/>
       <c r="G243" s="84"/>
@@ -11023,7 +11028,7 @@
       <c r="AJ243" s="84"/>
       <c r="AK243" s="84"/>
     </row>
-    <row r="244" spans="5:37" s="83" customFormat="1">
+    <row r="244" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E244" s="84"/>
       <c r="F244" s="84"/>
       <c r="G244" s="84"/>
@@ -11058,7 +11063,7 @@
       <c r="AJ244" s="84"/>
       <c r="AK244" s="84"/>
     </row>
-    <row r="245" spans="5:37" s="83" customFormat="1">
+    <row r="245" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E245" s="84"/>
       <c r="F245" s="84"/>
       <c r="G245" s="84"/>
@@ -11093,7 +11098,7 @@
       <c r="AJ245" s="84"/>
       <c r="AK245" s="84"/>
     </row>
-    <row r="246" spans="5:37" s="83" customFormat="1">
+    <row r="246" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E246" s="84"/>
       <c r="F246" s="84"/>
       <c r="G246" s="84"/>
@@ -11128,7 +11133,7 @@
       <c r="AJ246" s="84"/>
       <c r="AK246" s="84"/>
     </row>
-    <row r="247" spans="5:37" s="83" customFormat="1">
+    <row r="247" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E247" s="84"/>
       <c r="F247" s="84"/>
       <c r="G247" s="84"/>
@@ -11163,7 +11168,7 @@
       <c r="AJ247" s="84"/>
       <c r="AK247" s="84"/>
     </row>
-    <row r="248" spans="5:37" s="83" customFormat="1">
+    <row r="248" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E248" s="84"/>
       <c r="F248" s="84"/>
       <c r="G248" s="84"/>
@@ -11198,7 +11203,7 @@
       <c r="AJ248" s="84"/>
       <c r="AK248" s="84"/>
     </row>
-    <row r="249" spans="5:37" s="83" customFormat="1">
+    <row r="249" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E249" s="84"/>
       <c r="F249" s="84"/>
       <c r="G249" s="84"/>
@@ -11233,7 +11238,7 @@
       <c r="AJ249" s="84"/>
       <c r="AK249" s="84"/>
     </row>
-    <row r="250" spans="5:37" s="83" customFormat="1">
+    <row r="250" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E250" s="84"/>
       <c r="F250" s="84"/>
       <c r="G250" s="84"/>
@@ -11268,7 +11273,7 @@
       <c r="AJ250" s="84"/>
       <c r="AK250" s="84"/>
     </row>
-    <row r="251" spans="5:37" s="83" customFormat="1">
+    <row r="251" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E251" s="84"/>
       <c r="F251" s="84"/>
       <c r="G251" s="84"/>
@@ -11303,7 +11308,7 @@
       <c r="AJ251" s="84"/>
       <c r="AK251" s="84"/>
     </row>
-    <row r="252" spans="5:37" s="83" customFormat="1">
+    <row r="252" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E252" s="84"/>
       <c r="F252" s="84"/>
       <c r="G252" s="84"/>
@@ -11338,7 +11343,7 @@
       <c r="AJ252" s="84"/>
       <c r="AK252" s="84"/>
     </row>
-    <row r="253" spans="5:37" s="83" customFormat="1">
+    <row r="253" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E253" s="84"/>
       <c r="F253" s="84"/>
       <c r="G253" s="84"/>
@@ -11373,7 +11378,7 @@
       <c r="AJ253" s="84"/>
       <c r="AK253" s="84"/>
     </row>
-    <row r="254" spans="5:37" s="83" customFormat="1">
+    <row r="254" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E254" s="84"/>
       <c r="F254" s="84"/>
       <c r="G254" s="84"/>
@@ -11408,7 +11413,7 @@
       <c r="AJ254" s="84"/>
       <c r="AK254" s="84"/>
     </row>
-    <row r="255" spans="5:37" s="83" customFormat="1">
+    <row r="255" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E255" s="84"/>
       <c r="F255" s="84"/>
       <c r="G255" s="84"/>
@@ -11443,7 +11448,7 @@
       <c r="AJ255" s="84"/>
       <c r="AK255" s="84"/>
     </row>
-    <row r="256" spans="5:37" s="83" customFormat="1">
+    <row r="256" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E256" s="84"/>
       <c r="F256" s="84"/>
       <c r="G256" s="84"/>
@@ -11478,7 +11483,7 @@
       <c r="AJ256" s="84"/>
       <c r="AK256" s="84"/>
     </row>
-    <row r="257" spans="5:37" s="83" customFormat="1">
+    <row r="257" spans="5:37" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E257" s="84"/>
       <c r="F257" s="84"/>
       <c r="G257" s="84"/>
@@ -11513,7 +11518,7 @@
       <c r="AJ257" s="84"/>
       <c r="AK257" s="84"/>
     </row>
-    <row r="258" spans="5:37" s="39" customFormat="1">
+    <row r="258" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E258" s="110"/>
       <c r="F258" s="110"/>
       <c r="G258" s="110"/>
@@ -11548,7 +11553,7 @@
       <c r="AJ258" s="110"/>
       <c r="AK258" s="110"/>
     </row>
-    <row r="259" spans="5:37" s="39" customFormat="1">
+    <row r="259" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E259" s="110"/>
       <c r="F259" s="110"/>
       <c r="G259" s="110"/>
@@ -11583,7 +11588,7 @@
       <c r="AJ259" s="110"/>
       <c r="AK259" s="110"/>
     </row>
-    <row r="260" spans="5:37" s="39" customFormat="1">
+    <row r="260" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E260" s="110"/>
       <c r="F260" s="110"/>
       <c r="G260" s="110"/>
@@ -11618,7 +11623,7 @@
       <c r="AJ260" s="110"/>
       <c r="AK260" s="110"/>
     </row>
-    <row r="261" spans="5:37" s="39" customFormat="1">
+    <row r="261" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E261" s="110"/>
       <c r="F261" s="110"/>
       <c r="G261" s="110"/>
@@ -11653,7 +11658,7 @@
       <c r="AJ261" s="110"/>
       <c r="AK261" s="110"/>
     </row>
-    <row r="262" spans="5:37" s="39" customFormat="1">
+    <row r="262" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E262" s="110"/>
       <c r="F262" s="110"/>
       <c r="G262" s="110"/>
@@ -11688,7 +11693,7 @@
       <c r="AJ262" s="110"/>
       <c r="AK262" s="110"/>
     </row>
-    <row r="263" spans="5:37" s="39" customFormat="1">
+    <row r="263" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E263" s="110"/>
       <c r="F263" s="110"/>
       <c r="G263" s="110"/>
@@ -11723,7 +11728,7 @@
       <c r="AJ263" s="110"/>
       <c r="AK263" s="110"/>
     </row>
-    <row r="264" spans="5:37" s="39" customFormat="1">
+    <row r="264" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E264" s="110"/>
       <c r="F264" s="110"/>
       <c r="G264" s="110"/>
@@ -11758,7 +11763,7 @@
       <c r="AJ264" s="110"/>
       <c r="AK264" s="110"/>
     </row>
-    <row r="265" spans="5:37" s="39" customFormat="1">
+    <row r="265" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E265" s="110"/>
       <c r="F265" s="110"/>
       <c r="G265" s="110"/>
@@ -11793,7 +11798,7 @@
       <c r="AJ265" s="110"/>
       <c r="AK265" s="110"/>
     </row>
-    <row r="266" spans="5:37" s="39" customFormat="1">
+    <row r="266" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E266" s="110"/>
       <c r="F266" s="110"/>
       <c r="G266" s="110"/>
@@ -11828,7 +11833,7 @@
       <c r="AJ266" s="110"/>
       <c r="AK266" s="110"/>
     </row>
-    <row r="267" spans="5:37" s="39" customFormat="1">
+    <row r="267" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E267" s="110"/>
       <c r="F267" s="110"/>
       <c r="G267" s="110"/>
@@ -11863,7 +11868,7 @@
       <c r="AJ267" s="110"/>
       <c r="AK267" s="110"/>
     </row>
-    <row r="268" spans="5:37" s="39" customFormat="1">
+    <row r="268" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E268" s="110"/>
       <c r="F268" s="110"/>
       <c r="G268" s="110"/>
@@ -11898,7 +11903,7 @@
       <c r="AJ268" s="110"/>
       <c r="AK268" s="110"/>
     </row>
-    <row r="269" spans="5:37" s="39" customFormat="1">
+    <row r="269" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E269" s="110"/>
       <c r="F269" s="110"/>
       <c r="G269" s="110"/>
@@ -11933,7 +11938,7 @@
       <c r="AJ269" s="110"/>
       <c r="AK269" s="110"/>
     </row>
-    <row r="270" spans="5:37" s="39" customFormat="1">
+    <row r="270" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E270" s="110"/>
       <c r="F270" s="110"/>
       <c r="G270" s="110"/>
@@ -11968,7 +11973,7 @@
       <c r="AJ270" s="110"/>
       <c r="AK270" s="110"/>
     </row>
-    <row r="271" spans="5:37" s="39" customFormat="1">
+    <row r="271" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E271" s="110"/>
       <c r="F271" s="110"/>
       <c r="G271" s="110"/>
@@ -12003,7 +12008,7 @@
       <c r="AJ271" s="110"/>
       <c r="AK271" s="110"/>
     </row>
-    <row r="272" spans="5:37" s="39" customFormat="1">
+    <row r="272" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E272" s="110"/>
       <c r="F272" s="110"/>
       <c r="G272" s="110"/>
@@ -12038,7 +12043,7 @@
       <c r="AJ272" s="110"/>
       <c r="AK272" s="110"/>
     </row>
-    <row r="273" spans="5:37" s="39" customFormat="1">
+    <row r="273" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E273" s="110"/>
       <c r="F273" s="110"/>
       <c r="G273" s="110"/>
@@ -12073,7 +12078,7 @@
       <c r="AJ273" s="110"/>
       <c r="AK273" s="110"/>
     </row>
-    <row r="274" spans="5:37" s="39" customFormat="1">
+    <row r="274" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E274" s="110"/>
       <c r="F274" s="110"/>
       <c r="G274" s="110"/>
@@ -12108,7 +12113,7 @@
       <c r="AJ274" s="110"/>
       <c r="AK274" s="110"/>
     </row>
-    <row r="275" spans="5:37" s="39" customFormat="1">
+    <row r="275" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E275" s="110"/>
       <c r="F275" s="110"/>
       <c r="G275" s="110"/>
@@ -12143,7 +12148,7 @@
       <c r="AJ275" s="110"/>
       <c r="AK275" s="110"/>
     </row>
-    <row r="276" spans="5:37" s="39" customFormat="1">
+    <row r="276" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E276" s="110"/>
       <c r="F276" s="110"/>
       <c r="G276" s="110"/>
@@ -12178,7 +12183,7 @@
       <c r="AJ276" s="110"/>
       <c r="AK276" s="110"/>
     </row>
-    <row r="277" spans="5:37" s="39" customFormat="1">
+    <row r="277" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E277" s="110"/>
       <c r="F277" s="110"/>
       <c r="G277" s="110"/>
@@ -12213,7 +12218,7 @@
       <c r="AJ277" s="110"/>
       <c r="AK277" s="110"/>
     </row>
-    <row r="278" spans="5:37" s="39" customFormat="1">
+    <row r="278" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E278" s="110"/>
       <c r="F278" s="110"/>
       <c r="G278" s="110"/>
@@ -12248,7 +12253,7 @@
       <c r="AJ278" s="110"/>
       <c r="AK278" s="110"/>
     </row>
-    <row r="279" spans="5:37" s="39" customFormat="1">
+    <row r="279" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E279" s="110"/>
       <c r="F279" s="110"/>
       <c r="G279" s="110"/>
@@ -12283,7 +12288,7 @@
       <c r="AJ279" s="110"/>
       <c r="AK279" s="110"/>
     </row>
-    <row r="280" spans="5:37" s="39" customFormat="1">
+    <row r="280" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E280" s="110"/>
       <c r="F280" s="110"/>
       <c r="G280" s="110"/>
@@ -12318,7 +12323,7 @@
       <c r="AJ280" s="110"/>
       <c r="AK280" s="110"/>
     </row>
-    <row r="281" spans="5:37" s="39" customFormat="1">
+    <row r="281" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E281" s="110"/>
       <c r="F281" s="110"/>
       <c r="G281" s="110"/>
@@ -12353,7 +12358,7 @@
       <c r="AJ281" s="110"/>
       <c r="AK281" s="110"/>
     </row>
-    <row r="282" spans="5:37" s="39" customFormat="1">
+    <row r="282" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E282" s="110"/>
       <c r="F282" s="110"/>
       <c r="G282" s="110"/>
@@ -12388,7 +12393,7 @@
       <c r="AJ282" s="110"/>
       <c r="AK282" s="110"/>
     </row>
-    <row r="283" spans="5:37" s="39" customFormat="1">
+    <row r="283" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E283" s="110"/>
       <c r="F283" s="110"/>
       <c r="G283" s="110"/>
@@ -12423,7 +12428,7 @@
       <c r="AJ283" s="110"/>
       <c r="AK283" s="110"/>
     </row>
-    <row r="284" spans="5:37" s="39" customFormat="1">
+    <row r="284" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E284" s="110"/>
       <c r="F284" s="110"/>
       <c r="G284" s="110"/>
@@ -12458,7 +12463,7 @@
       <c r="AJ284" s="110"/>
       <c r="AK284" s="110"/>
     </row>
-    <row r="285" spans="5:37" s="39" customFormat="1">
+    <row r="285" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E285" s="110"/>
       <c r="F285" s="110"/>
       <c r="G285" s="110"/>
@@ -12493,7 +12498,7 @@
       <c r="AJ285" s="110"/>
       <c r="AK285" s="110"/>
     </row>
-    <row r="286" spans="5:37" s="39" customFormat="1">
+    <row r="286" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E286" s="110"/>
       <c r="F286" s="110"/>
       <c r="G286" s="110"/>
@@ -12528,7 +12533,7 @@
       <c r="AJ286" s="110"/>
       <c r="AK286" s="110"/>
     </row>
-    <row r="287" spans="5:37" s="39" customFormat="1">
+    <row r="287" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E287" s="110"/>
       <c r="F287" s="110"/>
       <c r="G287" s="110"/>
@@ -12563,7 +12568,7 @@
       <c r="AJ287" s="110"/>
       <c r="AK287" s="110"/>
     </row>
-    <row r="288" spans="5:37" s="39" customFormat="1">
+    <row r="288" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E288" s="110"/>
       <c r="F288" s="110"/>
       <c r="G288" s="110"/>
@@ -12598,7 +12603,7 @@
       <c r="AJ288" s="110"/>
       <c r="AK288" s="110"/>
     </row>
-    <row r="289" spans="5:37" s="39" customFormat="1">
+    <row r="289" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E289" s="110"/>
       <c r="F289" s="110"/>
       <c r="G289" s="110"/>
@@ -12633,7 +12638,7 @@
       <c r="AJ289" s="110"/>
       <c r="AK289" s="110"/>
     </row>
-    <row r="290" spans="5:37" s="39" customFormat="1">
+    <row r="290" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E290" s="110"/>
       <c r="F290" s="110"/>
       <c r="G290" s="110"/>
@@ -12668,7 +12673,7 @@
       <c r="AJ290" s="110"/>
       <c r="AK290" s="110"/>
     </row>
-    <row r="291" spans="5:37" s="39" customFormat="1">
+    <row r="291" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E291" s="110"/>
       <c r="F291" s="110"/>
       <c r="G291" s="110"/>
@@ -12703,7 +12708,7 @@
       <c r="AJ291" s="110"/>
       <c r="AK291" s="110"/>
     </row>
-    <row r="292" spans="5:37" s="39" customFormat="1">
+    <row r="292" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E292" s="110"/>
       <c r="F292" s="110"/>
       <c r="G292" s="110"/>
@@ -12738,7 +12743,7 @@
       <c r="AJ292" s="110"/>
       <c r="AK292" s="110"/>
     </row>
-    <row r="293" spans="5:37" s="39" customFormat="1">
+    <row r="293" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E293" s="110"/>
       <c r="F293" s="110"/>
       <c r="G293" s="110"/>
@@ -12773,7 +12778,7 @@
       <c r="AJ293" s="110"/>
       <c r="AK293" s="110"/>
     </row>
-    <row r="294" spans="5:37" s="39" customFormat="1">
+    <row r="294" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E294" s="110"/>
       <c r="F294" s="110"/>
       <c r="G294" s="110"/>
@@ -12808,7 +12813,7 @@
       <c r="AJ294" s="110"/>
       <c r="AK294" s="110"/>
     </row>
-    <row r="295" spans="5:37" s="39" customFormat="1">
+    <row r="295" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E295" s="110"/>
       <c r="F295" s="110"/>
       <c r="G295" s="110"/>
@@ -12843,7 +12848,7 @@
       <c r="AJ295" s="110"/>
       <c r="AK295" s="110"/>
     </row>
-    <row r="296" spans="5:37" s="39" customFormat="1">
+    <row r="296" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E296" s="110"/>
       <c r="F296" s="110"/>
       <c r="G296" s="110"/>
@@ -12878,7 +12883,7 @@
       <c r="AJ296" s="110"/>
       <c r="AK296" s="110"/>
     </row>
-    <row r="297" spans="5:37" s="39" customFormat="1">
+    <row r="297" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E297" s="110"/>
       <c r="F297" s="110"/>
       <c r="G297" s="110"/>
@@ -12913,7 +12918,7 @@
       <c r="AJ297" s="110"/>
       <c r="AK297" s="110"/>
     </row>
-    <row r="298" spans="5:37" s="39" customFormat="1">
+    <row r="298" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E298" s="110"/>
       <c r="F298" s="110"/>
       <c r="G298" s="110"/>
@@ -12948,7 +12953,7 @@
       <c r="AJ298" s="110"/>
       <c r="AK298" s="110"/>
     </row>
-    <row r="299" spans="5:37" s="39" customFormat="1">
+    <row r="299" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E299" s="110"/>
       <c r="F299" s="110"/>
       <c r="G299" s="110"/>
@@ -12983,7 +12988,7 @@
       <c r="AJ299" s="110"/>
       <c r="AK299" s="110"/>
     </row>
-    <row r="300" spans="5:37" s="39" customFormat="1">
+    <row r="300" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E300" s="110"/>
       <c r="F300" s="110"/>
       <c r="G300" s="110"/>
@@ -13018,7 +13023,7 @@
       <c r="AJ300" s="110"/>
       <c r="AK300" s="110"/>
     </row>
-    <row r="301" spans="5:37" s="39" customFormat="1">
+    <row r="301" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E301" s="110"/>
       <c r="F301" s="110"/>
       <c r="G301" s="110"/>
@@ -13053,7 +13058,7 @@
       <c r="AJ301" s="110"/>
       <c r="AK301" s="110"/>
     </row>
-    <row r="302" spans="5:37" s="39" customFormat="1">
+    <row r="302" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E302" s="110"/>
       <c r="F302" s="110"/>
       <c r="G302" s="110"/>
@@ -13088,7 +13093,7 @@
       <c r="AJ302" s="110"/>
       <c r="AK302" s="110"/>
     </row>
-    <row r="303" spans="5:37" s="39" customFormat="1">
+    <row r="303" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E303" s="110"/>
       <c r="F303" s="110"/>
       <c r="G303" s="110"/>
@@ -13123,7 +13128,7 @@
       <c r="AJ303" s="110"/>
       <c r="AK303" s="110"/>
     </row>
-    <row r="304" spans="5:37" s="39" customFormat="1">
+    <row r="304" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E304" s="110"/>
       <c r="F304" s="110"/>
       <c r="G304" s="110"/>
@@ -13158,7 +13163,7 @@
       <c r="AJ304" s="110"/>
       <c r="AK304" s="110"/>
     </row>
-    <row r="305" spans="5:37" s="39" customFormat="1">
+    <row r="305" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E305" s="110"/>
       <c r="F305" s="110"/>
       <c r="G305" s="110"/>
@@ -13193,7 +13198,7 @@
       <c r="AJ305" s="110"/>
       <c r="AK305" s="110"/>
     </row>
-    <row r="306" spans="5:37" s="39" customFormat="1">
+    <row r="306" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E306" s="110"/>
       <c r="F306" s="110"/>
       <c r="G306" s="110"/>
@@ -13228,7 +13233,7 @@
       <c r="AJ306" s="110"/>
       <c r="AK306" s="110"/>
     </row>
-    <row r="307" spans="5:37" s="39" customFormat="1">
+    <row r="307" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E307" s="110"/>
       <c r="F307" s="110"/>
       <c r="G307" s="110"/>
@@ -13263,7 +13268,7 @@
       <c r="AJ307" s="110"/>
       <c r="AK307" s="110"/>
     </row>
-    <row r="308" spans="5:37" s="39" customFormat="1">
+    <row r="308" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E308" s="110"/>
       <c r="F308" s="110"/>
       <c r="G308" s="110"/>
@@ -13298,7 +13303,7 @@
       <c r="AJ308" s="110"/>
       <c r="AK308" s="110"/>
     </row>
-    <row r="309" spans="5:37" s="39" customFormat="1">
+    <row r="309" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E309" s="110"/>
       <c r="F309" s="110"/>
       <c r="G309" s="110"/>
@@ -13333,7 +13338,7 @@
       <c r="AJ309" s="110"/>
       <c r="AK309" s="110"/>
     </row>
-    <row r="310" spans="5:37" s="39" customFormat="1">
+    <row r="310" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E310" s="110"/>
       <c r="F310" s="110"/>
       <c r="G310" s="110"/>
@@ -13368,7 +13373,7 @@
       <c r="AJ310" s="110"/>
       <c r="AK310" s="110"/>
     </row>
-    <row r="311" spans="5:37" s="39" customFormat="1">
+    <row r="311" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E311" s="110"/>
       <c r="F311" s="110"/>
       <c r="G311" s="110"/>
@@ -13403,7 +13408,7 @@
       <c r="AJ311" s="110"/>
       <c r="AK311" s="110"/>
     </row>
-    <row r="312" spans="5:37" s="39" customFormat="1">
+    <row r="312" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E312" s="110"/>
       <c r="F312" s="110"/>
       <c r="G312" s="110"/>
@@ -13438,7 +13443,7 @@
       <c r="AJ312" s="110"/>
       <c r="AK312" s="110"/>
     </row>
-    <row r="313" spans="5:37" s="39" customFormat="1">
+    <row r="313" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E313" s="110"/>
       <c r="F313" s="110"/>
       <c r="G313" s="110"/>
@@ -13473,7 +13478,7 @@
       <c r="AJ313" s="110"/>
       <c r="AK313" s="110"/>
     </row>
-    <row r="314" spans="5:37" s="39" customFormat="1">
+    <row r="314" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E314" s="110"/>
       <c r="F314" s="110"/>
       <c r="G314" s="110"/>
@@ -13508,7 +13513,7 @@
       <c r="AJ314" s="110"/>
       <c r="AK314" s="110"/>
     </row>
-    <row r="315" spans="5:37" s="39" customFormat="1">
+    <row r="315" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E315" s="110"/>
       <c r="F315" s="110"/>
       <c r="G315" s="110"/>
@@ -13543,7 +13548,7 @@
       <c r="AJ315" s="110"/>
       <c r="AK315" s="110"/>
     </row>
-    <row r="316" spans="5:37" s="39" customFormat="1">
+    <row r="316" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E316" s="110"/>
       <c r="F316" s="110"/>
       <c r="G316" s="110"/>
@@ -13578,7 +13583,7 @@
       <c r="AJ316" s="110"/>
       <c r="AK316" s="110"/>
     </row>
-    <row r="317" spans="5:37" s="39" customFormat="1">
+    <row r="317" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E317" s="110"/>
       <c r="F317" s="110"/>
       <c r="G317" s="110"/>
@@ -13613,7 +13618,7 @@
       <c r="AJ317" s="110"/>
       <c r="AK317" s="110"/>
     </row>
-    <row r="318" spans="5:37" s="39" customFormat="1">
+    <row r="318" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E318" s="110"/>
       <c r="F318" s="110"/>
       <c r="G318" s="110"/>
@@ -13648,7 +13653,7 @@
       <c r="AJ318" s="110"/>
       <c r="AK318" s="110"/>
     </row>
-    <row r="319" spans="5:37" s="39" customFormat="1">
+    <row r="319" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E319" s="110"/>
       <c r="F319" s="110"/>
       <c r="G319" s="110"/>
@@ -13683,7 +13688,7 @@
       <c r="AJ319" s="110"/>
       <c r="AK319" s="110"/>
     </row>
-    <row r="320" spans="5:37" s="39" customFormat="1">
+    <row r="320" spans="5:37" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E320" s="110"/>
       <c r="F320" s="110"/>
       <c r="G320" s="110"/>
@@ -13718,7 +13723,7 @@
       <c r="AJ320" s="110"/>
       <c r="AK320" s="110"/>
     </row>
-    <row r="321" spans="1:54" s="39" customFormat="1">
+    <row r="321" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A321" s="120"/>
       <c r="B321" s="120"/>
       <c r="C321" s="120"/>
@@ -13774,7 +13779,7 @@
       <c r="BA321" s="120"/>
       <c r="BB321" s="120"/>
     </row>
-    <row r="322" spans="1:54" s="39" customFormat="1">
+    <row r="322" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A322" s="120"/>
       <c r="B322" s="120"/>
       <c r="C322" s="120"/>
@@ -13830,7 +13835,7 @@
       <c r="BA322" s="120"/>
       <c r="BB322" s="120"/>
     </row>
-    <row r="323" spans="1:54" s="39" customFormat="1">
+    <row r="323" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A323" s="120"/>
       <c r="B323" s="120"/>
       <c r="C323" s="120"/>
@@ -13886,7 +13891,7 @@
       <c r="BA323" s="120"/>
       <c r="BB323" s="120"/>
     </row>
-    <row r="324" spans="1:54" s="39" customFormat="1">
+    <row r="324" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A324" s="120"/>
       <c r="B324" s="120"/>
       <c r="C324" s="120"/>
@@ -13942,7 +13947,7 @@
       <c r="BA324" s="120"/>
       <c r="BB324" s="120"/>
     </row>
-    <row r="325" spans="1:54" s="39" customFormat="1">
+    <row r="325" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A325" s="120"/>
       <c r="B325" s="120"/>
       <c r="C325" s="120"/>
@@ -13998,7 +14003,7 @@
       <c r="BA325" s="120"/>
       <c r="BB325" s="120"/>
     </row>
-    <row r="326" spans="1:54" s="39" customFormat="1">
+    <row r="326" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A326" s="120"/>
       <c r="B326" s="120"/>
       <c r="C326" s="120"/>
@@ -14054,7 +14059,7 @@
       <c r="BA326" s="120"/>
       <c r="BB326" s="120"/>
     </row>
-    <row r="327" spans="1:54" s="39" customFormat="1">
+    <row r="327" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A327" s="120"/>
       <c r="B327" s="120"/>
       <c r="C327" s="120"/>
@@ -14110,7 +14115,7 @@
       <c r="BA327" s="120"/>
       <c r="BB327" s="120"/>
     </row>
-    <row r="328" spans="1:54" s="39" customFormat="1">
+    <row r="328" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A328" s="120"/>
       <c r="B328" s="120"/>
       <c r="C328" s="120"/>
@@ -14166,7 +14171,7 @@
       <c r="BA328" s="120"/>
       <c r="BB328" s="120"/>
     </row>
-    <row r="329" spans="1:54" s="39" customFormat="1">
+    <row r="329" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A329" s="120"/>
       <c r="B329" s="120"/>
       <c r="C329" s="120"/>
@@ -14222,7 +14227,7 @@
       <c r="BA329" s="120"/>
       <c r="BB329" s="120"/>
     </row>
-    <row r="330" spans="1:54" s="39" customFormat="1">
+    <row r="330" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A330" s="120"/>
       <c r="B330" s="120"/>
       <c r="C330" s="120"/>
@@ -14278,7 +14283,7 @@
       <c r="BA330" s="120"/>
       <c r="BB330" s="120"/>
     </row>
-    <row r="331" spans="1:54" s="39" customFormat="1">
+    <row r="331" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A331" s="120"/>
       <c r="B331" s="120"/>
       <c r="C331" s="120"/>
@@ -14334,7 +14339,7 @@
       <c r="BA331" s="120"/>
       <c r="BB331" s="120"/>
     </row>
-    <row r="332" spans="1:54" s="39" customFormat="1">
+    <row r="332" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A332" s="120"/>
       <c r="B332" s="120"/>
       <c r="C332" s="120"/>
@@ -14390,7 +14395,7 @@
       <c r="BA332" s="120"/>
       <c r="BB332" s="120"/>
     </row>
-    <row r="333" spans="1:54" s="39" customFormat="1">
+    <row r="333" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A333" s="120"/>
       <c r="B333" s="120"/>
       <c r="C333" s="120"/>
@@ -14446,7 +14451,7 @@
       <c r="BA333" s="120"/>
       <c r="BB333" s="120"/>
     </row>
-    <row r="334" spans="1:54" s="39" customFormat="1">
+    <row r="334" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A334" s="120"/>
       <c r="B334" s="120"/>
       <c r="C334" s="120"/>
@@ -14502,7 +14507,7 @@
       <c r="BA334" s="120"/>
       <c r="BB334" s="120"/>
     </row>
-    <row r="335" spans="1:54" s="39" customFormat="1">
+    <row r="335" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A335" s="120"/>
       <c r="B335" s="120"/>
       <c r="C335" s="120"/>
@@ -14558,7 +14563,7 @@
       <c r="BA335" s="120"/>
       <c r="BB335" s="120"/>
     </row>
-    <row r="336" spans="1:54" s="39" customFormat="1">
+    <row r="336" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A336" s="87"/>
       <c r="B336" s="87"/>
       <c r="C336" s="87"/>
@@ -14614,7 +14619,7 @@
       <c r="BA336" s="87"/>
       <c r="BB336" s="87"/>
     </row>
-    <row r="337" spans="1:54" s="39" customFormat="1">
+    <row r="337" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A337" s="87"/>
       <c r="B337" s="87"/>
       <c r="C337" s="87"/>
@@ -14670,7 +14675,7 @@
       <c r="BA337" s="87"/>
       <c r="BB337" s="87"/>
     </row>
-    <row r="338" spans="1:54" s="39" customFormat="1">
+    <row r="338" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A338" s="87"/>
       <c r="B338" s="87"/>
       <c r="C338" s="87"/>
@@ -14726,7 +14731,7 @@
       <c r="BA338" s="87"/>
       <c r="BB338" s="87"/>
     </row>
-    <row r="339" spans="1:54" s="39" customFormat="1">
+    <row r="339" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A339" s="87"/>
       <c r="B339" s="87"/>
       <c r="C339" s="87"/>
@@ -14782,7 +14787,7 @@
       <c r="BA339" s="87"/>
       <c r="BB339" s="87"/>
     </row>
-    <row r="340" spans="1:54" s="39" customFormat="1">
+    <row r="340" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A340" s="87"/>
       <c r="B340" s="87"/>
       <c r="C340" s="87"/>
@@ -14838,7 +14843,7 @@
       <c r="BA340" s="87"/>
       <c r="BB340" s="87"/>
     </row>
-    <row r="341" spans="1:54" s="39" customFormat="1">
+    <row r="341" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A341" s="87"/>
       <c r="B341" s="87"/>
       <c r="C341" s="87"/>
@@ -14894,7 +14899,7 @@
       <c r="BA341" s="87"/>
       <c r="BB341" s="87"/>
     </row>
-    <row r="342" spans="1:54" s="39" customFormat="1">
+    <row r="342" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A342" s="87"/>
       <c r="B342" s="87"/>
       <c r="C342" s="87"/>
@@ -14950,7 +14955,7 @@
       <c r="BA342" s="87"/>
       <c r="BB342" s="87"/>
     </row>
-    <row r="343" spans="1:54" s="39" customFormat="1">
+    <row r="343" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A343" s="87"/>
       <c r="B343" s="87"/>
       <c r="C343" s="87"/>
@@ -15006,7 +15011,7 @@
       <c r="BA343" s="87"/>
       <c r="BB343" s="87"/>
     </row>
-    <row r="344" spans="1:54" s="39" customFormat="1">
+    <row r="344" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A344" s="87"/>
       <c r="B344" s="87"/>
       <c r="C344" s="87"/>
@@ -15062,7 +15067,7 @@
       <c r="BA344" s="87"/>
       <c r="BB344" s="87"/>
     </row>
-    <row r="345" spans="1:54" s="39" customFormat="1">
+    <row r="345" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A345" s="87"/>
       <c r="B345" s="87"/>
       <c r="C345" s="87"/>
@@ -15118,7 +15123,7 @@
       <c r="BA345" s="87"/>
       <c r="BB345" s="87"/>
     </row>
-    <row r="346" spans="1:54" s="39" customFormat="1">
+    <row r="346" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A346" s="87"/>
       <c r="B346" s="87"/>
       <c r="C346" s="87"/>
@@ -15174,7 +15179,7 @@
       <c r="BA346" s="87"/>
       <c r="BB346" s="87"/>
     </row>
-    <row r="347" spans="1:54" s="39" customFormat="1">
+    <row r="347" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A347" s="87"/>
       <c r="B347" s="87"/>
       <c r="C347" s="87"/>
@@ -15230,7 +15235,7 @@
       <c r="BA347" s="87"/>
       <c r="BB347" s="87"/>
     </row>
-    <row r="348" spans="1:54" s="39" customFormat="1">
+    <row r="348" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A348" s="87"/>
       <c r="B348" s="87"/>
       <c r="C348" s="87"/>
@@ -15286,7 +15291,7 @@
       <c r="BA348" s="87"/>
       <c r="BB348" s="87"/>
     </row>
-    <row r="349" spans="1:54" s="39" customFormat="1">
+    <row r="349" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A349" s="87"/>
       <c r="B349" s="87"/>
       <c r="C349" s="87"/>
@@ -15342,7 +15347,7 @@
       <c r="BA349" s="87"/>
       <c r="BB349" s="87"/>
     </row>
-    <row r="350" spans="1:54" s="39" customFormat="1">
+    <row r="350" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A350" s="87"/>
       <c r="B350" s="87"/>
       <c r="C350" s="87"/>
@@ -15398,7 +15403,7 @@
       <c r="BA350" s="87"/>
       <c r="BB350" s="87"/>
     </row>
-    <row r="351" spans="1:54" s="39" customFormat="1">
+    <row r="351" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A351" s="87"/>
       <c r="B351" s="87"/>
       <c r="C351" s="87"/>
@@ -15454,7 +15459,7 @@
       <c r="BA351" s="87"/>
       <c r="BB351" s="87"/>
     </row>
-    <row r="352" spans="1:54" s="39" customFormat="1">
+    <row r="352" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A352" s="87"/>
       <c r="B352" s="87"/>
       <c r="C352" s="87"/>
@@ -15510,7 +15515,7 @@
       <c r="BA352" s="87"/>
       <c r="BB352" s="87"/>
     </row>
-    <row r="353" spans="1:54" s="39" customFormat="1">
+    <row r="353" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A353" s="87"/>
       <c r="B353" s="87"/>
       <c r="C353" s="87"/>
@@ -15566,7 +15571,7 @@
       <c r="BA353" s="87"/>
       <c r="BB353" s="87"/>
     </row>
-    <row r="354" spans="1:54" s="39" customFormat="1">
+    <row r="354" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A354" s="87"/>
       <c r="B354" s="87"/>
       <c r="C354" s="87"/>
@@ -15622,7 +15627,7 @@
       <c r="BA354" s="87"/>
       <c r="BB354" s="87"/>
     </row>
-    <row r="355" spans="1:54" s="39" customFormat="1">
+    <row r="355" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A355" s="87"/>
       <c r="B355" s="87"/>
       <c r="C355" s="87"/>
@@ -15678,7 +15683,7 @@
       <c r="BA355" s="87"/>
       <c r="BB355" s="87"/>
     </row>
-    <row r="356" spans="1:54" s="39" customFormat="1">
+    <row r="356" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A356" s="87"/>
       <c r="B356" s="87"/>
       <c r="C356" s="87"/>
@@ -15734,7 +15739,7 @@
       <c r="BA356" s="87"/>
       <c r="BB356" s="87"/>
     </row>
-    <row r="357" spans="1:54" s="39" customFormat="1">
+    <row r="357" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A357" s="87"/>
       <c r="B357" s="87"/>
       <c r="C357" s="87"/>
@@ -15790,7 +15795,7 @@
       <c r="BA357" s="87"/>
       <c r="BB357" s="87"/>
     </row>
-    <row r="358" spans="1:54" s="39" customFormat="1">
+    <row r="358" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A358" s="87"/>
       <c r="B358" s="87"/>
       <c r="C358" s="87"/>
@@ -15846,7 +15851,7 @@
       <c r="BA358" s="87"/>
       <c r="BB358" s="87"/>
     </row>
-    <row r="359" spans="1:54" s="39" customFormat="1">
+    <row r="359" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A359" s="87"/>
       <c r="B359" s="87"/>
       <c r="C359" s="87"/>
@@ -15902,7 +15907,7 @@
       <c r="BA359" s="87"/>
       <c r="BB359" s="87"/>
     </row>
-    <row r="360" spans="1:54" s="39" customFormat="1">
+    <row r="360" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A360" s="87"/>
       <c r="B360" s="87"/>
       <c r="C360" s="87"/>
@@ -15958,7 +15963,7 @@
       <c r="BA360" s="87"/>
       <c r="BB360" s="87"/>
     </row>
-    <row r="361" spans="1:54" s="39" customFormat="1">
+    <row r="361" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A361" s="87"/>
       <c r="B361" s="87"/>
       <c r="C361" s="87"/>
@@ -16014,7 +16019,7 @@
       <c r="BA361" s="87"/>
       <c r="BB361" s="87"/>
     </row>
-    <row r="362" spans="1:54" s="39" customFormat="1">
+    <row r="362" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A362" s="87"/>
       <c r="B362" s="87"/>
       <c r="C362" s="87"/>
@@ -16070,7 +16075,7 @@
       <c r="BA362" s="87"/>
       <c r="BB362" s="87"/>
     </row>
-    <row r="363" spans="1:54" s="39" customFormat="1">
+    <row r="363" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A363" s="87"/>
       <c r="B363" s="87"/>
       <c r="C363" s="87"/>
@@ -16126,7 +16131,7 @@
       <c r="BA363" s="87"/>
       <c r="BB363" s="87"/>
     </row>
-    <row r="364" spans="1:54" s="39" customFormat="1">
+    <row r="364" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A364" s="87"/>
       <c r="B364" s="87"/>
       <c r="C364" s="87"/>
@@ -16182,7 +16187,7 @@
       <c r="BA364" s="87"/>
       <c r="BB364" s="87"/>
     </row>
-    <row r="365" spans="1:54" s="39" customFormat="1">
+    <row r="365" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A365" s="87"/>
       <c r="B365" s="87"/>
       <c r="C365" s="87"/>
@@ -16238,7 +16243,7 @@
       <c r="BA365" s="87"/>
       <c r="BB365" s="87"/>
     </row>
-    <row r="366" spans="1:54" s="39" customFormat="1">
+    <row r="366" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A366" s="87"/>
       <c r="B366" s="87"/>
       <c r="C366" s="87"/>
@@ -16294,7 +16299,7 @@
       <c r="BA366" s="87"/>
       <c r="BB366" s="87"/>
     </row>
-    <row r="367" spans="1:54" s="39" customFormat="1">
+    <row r="367" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A367" s="87"/>
       <c r="B367" s="87"/>
       <c r="C367" s="87"/>
@@ -16350,7 +16355,7 @@
       <c r="BA367" s="87"/>
       <c r="BB367" s="87"/>
     </row>
-    <row r="368" spans="1:54" s="39" customFormat="1">
+    <row r="368" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A368" s="87"/>
       <c r="B368" s="87"/>
       <c r="C368" s="87"/>
@@ -16406,7 +16411,7 @@
       <c r="BA368" s="87"/>
       <c r="BB368" s="87"/>
     </row>
-    <row r="369" spans="1:54" s="39" customFormat="1">
+    <row r="369" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A369" s="87"/>
       <c r="B369" s="87"/>
       <c r="C369" s="87"/>
@@ -16462,7 +16467,7 @@
       <c r="BA369" s="87"/>
       <c r="BB369" s="87"/>
     </row>
-    <row r="370" spans="1:54" s="39" customFormat="1">
+    <row r="370" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A370" s="87"/>
       <c r="B370" s="87"/>
       <c r="C370" s="87"/>
@@ -16518,7 +16523,7 @@
       <c r="BA370" s="87"/>
       <c r="BB370" s="87"/>
     </row>
-    <row r="371" spans="1:54" s="39" customFormat="1">
+    <row r="371" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A371" s="87"/>
       <c r="B371" s="87"/>
       <c r="C371" s="87"/>
@@ -16574,7 +16579,7 @@
       <c r="BA371" s="87"/>
       <c r="BB371" s="87"/>
     </row>
-    <row r="372" spans="1:54" s="39" customFormat="1">
+    <row r="372" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A372" s="87"/>
       <c r="B372" s="87"/>
       <c r="C372" s="87"/>
@@ -16630,7 +16635,7 @@
       <c r="BA372" s="87"/>
       <c r="BB372" s="87"/>
     </row>
-    <row r="373" spans="1:54" s="39" customFormat="1">
+    <row r="373" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A373" s="87"/>
       <c r="B373" s="87"/>
       <c r="C373" s="87"/>
@@ -16686,7 +16691,7 @@
       <c r="BA373" s="87"/>
       <c r="BB373" s="87"/>
     </row>
-    <row r="374" spans="1:54" s="39" customFormat="1">
+    <row r="374" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A374" s="87"/>
       <c r="B374" s="87"/>
       <c r="C374" s="87"/>
@@ -16742,7 +16747,7 @@
       <c r="BA374" s="87"/>
       <c r="BB374" s="87"/>
     </row>
-    <row r="375" spans="1:54" s="39" customFormat="1">
+    <row r="375" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A375" s="87"/>
       <c r="B375" s="87"/>
       <c r="C375" s="87"/>
@@ -16798,7 +16803,7 @@
       <c r="BA375" s="87"/>
       <c r="BB375" s="87"/>
     </row>
-    <row r="376" spans="1:54" s="39" customFormat="1">
+    <row r="376" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A376" s="87"/>
       <c r="B376" s="87"/>
       <c r="C376" s="87"/>
@@ -16854,7 +16859,7 @@
       <c r="BA376" s="87"/>
       <c r="BB376" s="87"/>
     </row>
-    <row r="377" spans="1:54" s="39" customFormat="1">
+    <row r="377" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A377" s="87"/>
       <c r="B377" s="87"/>
       <c r="C377" s="87"/>
@@ -16910,7 +16915,7 @@
       <c r="BA377" s="87"/>
       <c r="BB377" s="87"/>
     </row>
-    <row r="378" spans="1:54" s="39" customFormat="1">
+    <row r="378" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A378" s="87"/>
       <c r="B378" s="87"/>
       <c r="C378" s="87"/>
@@ -16966,7 +16971,7 @@
       <c r="BA378" s="87"/>
       <c r="BB378" s="87"/>
     </row>
-    <row r="379" spans="1:54" s="39" customFormat="1">
+    <row r="379" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A379" s="87"/>
       <c r="B379" s="87"/>
       <c r="C379" s="87"/>
@@ -17022,7 +17027,7 @@
       <c r="BA379" s="87"/>
       <c r="BB379" s="87"/>
     </row>
-    <row r="380" spans="1:54" s="39" customFormat="1">
+    <row r="380" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A380" s="87"/>
       <c r="B380" s="87"/>
       <c r="C380" s="87"/>
@@ -17078,7 +17083,7 @@
       <c r="BA380" s="87"/>
       <c r="BB380" s="87"/>
     </row>
-    <row r="381" spans="1:54" s="39" customFormat="1">
+    <row r="381" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A381" s="87"/>
       <c r="B381" s="87"/>
       <c r="C381" s="87"/>
@@ -17134,7 +17139,7 @@
       <c r="BA381" s="87"/>
       <c r="BB381" s="87"/>
     </row>
-    <row r="382" spans="1:54" s="39" customFormat="1">
+    <row r="382" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A382" s="87"/>
       <c r="B382" s="87"/>
       <c r="C382" s="87"/>
@@ -17190,7 +17195,7 @@
       <c r="BA382" s="87"/>
       <c r="BB382" s="87"/>
     </row>
-    <row r="383" spans="1:54" s="39" customFormat="1">
+    <row r="383" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A383" s="87"/>
       <c r="B383" s="87"/>
       <c r="C383" s="87"/>
@@ -17246,7 +17251,7 @@
       <c r="BA383" s="87"/>
       <c r="BB383" s="87"/>
     </row>
-    <row r="384" spans="1:54" s="39" customFormat="1">
+    <row r="384" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A384" s="87"/>
       <c r="B384" s="87"/>
       <c r="C384" s="87"/>
@@ -17302,7 +17307,7 @@
       <c r="BA384" s="87"/>
       <c r="BB384" s="87"/>
     </row>
-    <row r="385" spans="1:54" s="39" customFormat="1">
+    <row r="385" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A385" s="87"/>
       <c r="B385" s="87"/>
       <c r="C385" s="87"/>
@@ -17358,7 +17363,7 @@
       <c r="BA385" s="87"/>
       <c r="BB385" s="87"/>
     </row>
-    <row r="386" spans="1:54" s="39" customFormat="1">
+    <row r="386" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A386" s="87"/>
       <c r="B386" s="87"/>
       <c r="C386" s="87"/>
@@ -17414,7 +17419,7 @@
       <c r="BA386" s="87"/>
       <c r="BB386" s="87"/>
     </row>
-    <row r="387" spans="1:54" s="39" customFormat="1">
+    <row r="387" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A387" s="87"/>
       <c r="B387" s="87"/>
       <c r="C387" s="87"/>
@@ -17470,7 +17475,7 @@
       <c r="BA387" s="87"/>
       <c r="BB387" s="87"/>
     </row>
-    <row r="388" spans="1:54" s="39" customFormat="1">
+    <row r="388" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A388" s="87"/>
       <c r="B388" s="87"/>
       <c r="C388" s="87"/>
@@ -17526,7 +17531,7 @@
       <c r="BA388" s="87"/>
       <c r="BB388" s="87"/>
     </row>
-    <row r="389" spans="1:54" s="39" customFormat="1">
+    <row r="389" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A389" s="87"/>
       <c r="B389" s="87"/>
       <c r="C389" s="87"/>
@@ -17582,7 +17587,7 @@
       <c r="BA389" s="87"/>
       <c r="BB389" s="87"/>
     </row>
-    <row r="390" spans="1:54" s="39" customFormat="1">
+    <row r="390" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A390" s="87"/>
       <c r="B390" s="87"/>
       <c r="C390" s="87"/>
@@ -17638,7 +17643,7 @@
       <c r="BA390" s="87"/>
       <c r="BB390" s="87"/>
     </row>
-    <row r="391" spans="1:54" s="39" customFormat="1">
+    <row r="391" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A391" s="87"/>
       <c r="B391" s="87"/>
       <c r="C391" s="87"/>
@@ -17694,7 +17699,7 @@
       <c r="BA391" s="87"/>
       <c r="BB391" s="87"/>
     </row>
-    <row r="392" spans="1:54" s="39" customFormat="1">
+    <row r="392" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A392" s="87"/>
       <c r="B392" s="87"/>
       <c r="C392" s="87"/>
@@ -17750,7 +17755,7 @@
       <c r="BA392" s="87"/>
       <c r="BB392" s="87"/>
     </row>
-    <row r="393" spans="1:54" s="39" customFormat="1">
+    <row r="393" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A393" s="87"/>
       <c r="B393" s="87"/>
       <c r="C393" s="87"/>
@@ -17806,7 +17811,7 @@
       <c r="BA393" s="87"/>
       <c r="BB393" s="87"/>
     </row>
-    <row r="394" spans="1:54" s="39" customFormat="1">
+    <row r="394" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A394" s="87"/>
       <c r="B394" s="87"/>
       <c r="C394" s="87"/>
@@ -17862,7 +17867,7 @@
       <c r="BA394" s="87"/>
       <c r="BB394" s="87"/>
     </row>
-    <row r="395" spans="1:54" s="39" customFormat="1">
+    <row r="395" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A395" s="87"/>
       <c r="B395" s="87"/>
       <c r="C395" s="87"/>
@@ -17918,7 +17923,7 @@
       <c r="BA395" s="87"/>
       <c r="BB395" s="87"/>
     </row>
-    <row r="396" spans="1:54" s="39" customFormat="1">
+    <row r="396" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A396" s="87"/>
       <c r="B396" s="87"/>
       <c r="C396" s="87"/>
@@ -17974,7 +17979,7 @@
       <c r="BA396" s="87"/>
       <c r="BB396" s="87"/>
     </row>
-    <row r="397" spans="1:54" s="39" customFormat="1">
+    <row r="397" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A397" s="87"/>
       <c r="B397" s="87"/>
       <c r="C397" s="87"/>
@@ -18030,7 +18035,7 @@
       <c r="BA397" s="87"/>
       <c r="BB397" s="87"/>
     </row>
-    <row r="398" spans="1:54" s="39" customFormat="1">
+    <row r="398" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A398" s="87"/>
       <c r="B398" s="87"/>
       <c r="C398" s="87"/>
@@ -18086,7 +18091,7 @@
       <c r="BA398" s="87"/>
       <c r="BB398" s="87"/>
     </row>
-    <row r="399" spans="1:54" s="39" customFormat="1">
+    <row r="399" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A399" s="87"/>
       <c r="B399" s="87"/>
       <c r="C399" s="87"/>
@@ -18142,7 +18147,7 @@
       <c r="BA399" s="87"/>
       <c r="BB399" s="87"/>
     </row>
-    <row r="400" spans="1:54" s="39" customFormat="1">
+    <row r="400" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A400" s="87"/>
       <c r="B400" s="87"/>
       <c r="C400" s="87"/>
@@ -18198,7 +18203,7 @@
       <c r="BA400" s="87"/>
       <c r="BB400" s="87"/>
     </row>
-    <row r="401" spans="1:54" s="39" customFormat="1">
+    <row r="401" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A401" s="87"/>
       <c r="B401" s="87"/>
       <c r="C401" s="87"/>
@@ -18254,7 +18259,7 @@
       <c r="BA401" s="87"/>
       <c r="BB401" s="87"/>
     </row>
-    <row r="402" spans="1:54" s="39" customFormat="1">
+    <row r="402" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A402" s="87"/>
       <c r="B402" s="87"/>
       <c r="C402" s="87"/>
@@ -18310,7 +18315,7 @@
       <c r="BA402" s="87"/>
       <c r="BB402" s="87"/>
     </row>
-    <row r="403" spans="1:54" s="39" customFormat="1">
+    <row r="403" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A403" s="87"/>
       <c r="B403" s="87"/>
       <c r="C403" s="87"/>
@@ -18366,7 +18371,7 @@
       <c r="BA403" s="87"/>
       <c r="BB403" s="87"/>
     </row>
-    <row r="404" spans="1:54" s="39" customFormat="1">
+    <row r="404" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A404" s="87"/>
       <c r="B404" s="87"/>
       <c r="C404" s="87"/>
@@ -18422,7 +18427,7 @@
       <c r="BA404" s="87"/>
       <c r="BB404" s="87"/>
     </row>
-    <row r="405" spans="1:54" s="39" customFormat="1">
+    <row r="405" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A405" s="87"/>
       <c r="B405" s="87"/>
       <c r="C405" s="87"/>
@@ -18478,7 +18483,7 @@
       <c r="BA405" s="87"/>
       <c r="BB405" s="87"/>
     </row>
-    <row r="406" spans="1:54" s="39" customFormat="1">
+    <row r="406" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A406" s="87"/>
       <c r="B406" s="87"/>
       <c r="C406" s="87"/>
@@ -18534,7 +18539,7 @@
       <c r="BA406" s="87"/>
       <c r="BB406" s="87"/>
     </row>
-    <row r="407" spans="1:54" s="39" customFormat="1">
+    <row r="407" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A407" s="87"/>
       <c r="B407" s="87"/>
       <c r="C407" s="87"/>
@@ -18590,7 +18595,7 @@
       <c r="BA407" s="87"/>
       <c r="BB407" s="87"/>
     </row>
-    <row r="408" spans="1:54" s="39" customFormat="1">
+    <row r="408" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A408" s="87"/>
       <c r="B408" s="87"/>
       <c r="C408" s="87"/>
@@ -18646,7 +18651,7 @@
       <c r="BA408" s="87"/>
       <c r="BB408" s="87"/>
     </row>
-    <row r="409" spans="1:54" s="39" customFormat="1">
+    <row r="409" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A409" s="87"/>
       <c r="B409" s="87"/>
       <c r="C409" s="87"/>
@@ -18702,7 +18707,7 @@
       <c r="BA409" s="87"/>
       <c r="BB409" s="87"/>
     </row>
-    <row r="410" spans="1:54" s="39" customFormat="1">
+    <row r="410" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A410" s="87"/>
       <c r="B410" s="87"/>
       <c r="C410" s="87"/>
@@ -18758,7 +18763,7 @@
       <c r="BA410" s="87"/>
       <c r="BB410" s="87"/>
     </row>
-    <row r="411" spans="1:54" s="39" customFormat="1">
+    <row r="411" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A411" s="87"/>
       <c r="B411" s="87"/>
       <c r="C411" s="87"/>
@@ -18814,7 +18819,7 @@
       <c r="BA411" s="87"/>
       <c r="BB411" s="87"/>
     </row>
-    <row r="412" spans="1:54" s="39" customFormat="1">
+    <row r="412" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A412" s="87"/>
       <c r="B412" s="87"/>
       <c r="C412" s="87"/>
@@ -18870,7 +18875,7 @@
       <c r="BA412" s="87"/>
       <c r="BB412" s="87"/>
     </row>
-    <row r="413" spans="1:54" s="39" customFormat="1">
+    <row r="413" spans="1:54" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A413" s="87"/>
       <c r="B413" s="87"/>
       <c r="C413" s="87"/>

</xml_diff>